<commit_message>
Update outputs from code/analysis/08_spatial_registration
</commit_message>
<xml_diff>
--- a/processed-data/rdata/spe/08_spatial_registration/bayesSpace_layer_cor_annotations.xlsx
+++ b/processed-data/rdata/spe/08_spatial_registration/bayesSpace_layer_cor_annotations.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="219">
   <si>
     <t>data</t>
   </si>
@@ -94,67 +94,67 @@
     <t>WM</t>
   </si>
   <si>
+    <t>L3</t>
+  </si>
+  <si>
+    <t>L4</t>
+  </si>
+  <si>
     <t>L2</t>
   </si>
   <si>
-    <t>L3</t>
-  </si>
-  <si>
-    <t>L4</t>
+    <t>L5/6</t>
   </si>
   <si>
     <t>L6/WM</t>
   </si>
   <si>
-    <t>L1/2</t>
-  </si>
-  <si>
-    <t>Sp7D1 ~ L1</t>
-  </si>
-  <si>
-    <t>Sp7D2 ~ L2/3</t>
-  </si>
-  <si>
-    <t>Sp7D3 ~ L3/4</t>
-  </si>
-  <si>
-    <t>Sp7D4 ~ L5</t>
-  </si>
-  <si>
-    <t>Sp7D6 ~ L6</t>
-  </si>
-  <si>
-    <t>Sp7D5 ~ WM</t>
-  </si>
-  <si>
-    <t>Sp7D7 ~ WM</t>
-  </si>
-  <si>
-    <t>Sp9D1 ~ L1</t>
-  </si>
-  <si>
-    <t>Sp9D2 ~ L1</t>
-  </si>
-  <si>
-    <t>Sp9D3 ~ L2</t>
-  </si>
-  <si>
-    <t>Sp9D5 ~ L3</t>
-  </si>
-  <si>
-    <t>Sp9D8 ~ L4</t>
-  </si>
-  <si>
-    <t>Sp9D4 ~ L5</t>
-  </si>
-  <si>
-    <t>Sp9D7 ~ L6</t>
-  </si>
-  <si>
-    <t>Sp9D9 ~ L6/WM</t>
-  </si>
-  <si>
-    <t>Sp9D6 ~ WM</t>
+    <t>Sp07D01 ~ L1</t>
+  </si>
+  <si>
+    <t>Sp07D02 ~ L2/3</t>
+  </si>
+  <si>
+    <t>Sp07D03 ~ L3/4</t>
+  </si>
+  <si>
+    <t>Sp07D04 ~ L5</t>
+  </si>
+  <si>
+    <t>Sp07D06 ~ L6</t>
+  </si>
+  <si>
+    <t>Sp07D05 ~ WM</t>
+  </si>
+  <si>
+    <t>Sp07D07 ~ WM</t>
+  </si>
+  <si>
+    <t>Sp09D01 ~ L1</t>
+  </si>
+  <si>
+    <t>Sp09D02 ~ L1</t>
+  </si>
+  <si>
+    <t>Sp09D03 ~ L2/3</t>
+  </si>
+  <si>
+    <t>Sp09D05 ~ L3</t>
+  </si>
+  <si>
+    <t>Sp09D08 ~ L4</t>
+  </si>
+  <si>
+    <t>Sp09D04 ~ L5</t>
+  </si>
+  <si>
+    <t>Sp09D07 ~ L6</t>
+  </si>
+  <si>
+    <t>Sp09D06 ~ WM</t>
+  </si>
+  <si>
+    <t>Sp09D09 ~ WM</t>
   </si>
   <si>
     <t>Sp16D01 ~ L1</t>
@@ -169,12 +169,12 @@
     <t>Sp16D08 ~ L2</t>
   </si>
   <si>
+    <t>Sp16D10 ~ L2/3</t>
+  </si>
+  <si>
     <t>Sp16D03 ~ L3</t>
   </si>
   <si>
-    <t>Sp16D10 ~ L3</t>
-  </si>
-  <si>
     <t>Sp16D09 ~ L3/4</t>
   </si>
   <si>
@@ -193,18 +193,21 @@
     <t>Sp16D12 ~ L6</t>
   </si>
   <si>
-    <t>Sp16D13 ~ L6/WM</t>
-  </si>
-  <si>
     <t>Sp16D06 ~ WM</t>
   </si>
   <si>
     <t>Sp16D11 ~ WM</t>
   </si>
   <si>
+    <t>Sp16D13 ~ WM</t>
+  </si>
+  <si>
     <t>Sp16D15 ~ WM</t>
   </si>
   <si>
+    <t>Sp28D11 ~ L1</t>
+  </si>
+  <si>
     <t>Sp28D12 ~ L1</t>
   </si>
   <si>
@@ -220,9 +223,6 @@
     <t>Sp28D27 ~ L1</t>
   </si>
   <si>
-    <t>Sp28D11 ~ L1/2</t>
-  </si>
-  <si>
     <t>Sp28D09 ~ L2</t>
   </si>
   <si>
@@ -241,15 +241,15 @@
     <t>Sp28D10 ~ L3/4</t>
   </si>
   <si>
+    <t>Sp28D24 ~ L3/4</t>
+  </si>
+  <si>
     <t>Sp28D05 ~ L4</t>
   </si>
   <si>
     <t>Sp28D22 ~ L4</t>
   </si>
   <si>
-    <t>Sp28D24 ~ L4</t>
-  </si>
-  <si>
     <t>Sp28D25 ~ L4</t>
   </si>
   <si>
@@ -259,15 +259,15 @@
     <t>Sp28D13 ~ L5</t>
   </si>
   <si>
+    <t>Sp28D19 ~ L5/6</t>
+  </si>
+  <si>
     <t>Sp28D07 ~ L6</t>
   </si>
   <si>
     <t>Sp28D14 ~ L6</t>
   </si>
   <si>
-    <t>Sp28D19 ~ L6</t>
-  </si>
-  <si>
     <t>Sp28D16 ~ L6/WM</t>
   </si>
   <si>
@@ -283,52 +283,52 @@
     <t>Sp28D28 ~ WM</t>
   </si>
   <si>
-    <t>L1 Sp7D1</t>
-  </si>
-  <si>
-    <t>L2/3 Sp7D2</t>
-  </si>
-  <si>
-    <t>L3/4 Sp7D3</t>
-  </si>
-  <si>
-    <t>L5 Sp7D4</t>
-  </si>
-  <si>
-    <t>L6 Sp7D6</t>
-  </si>
-  <si>
-    <t>WM Sp7D5</t>
-  </si>
-  <si>
-    <t>WM Sp7D7</t>
-  </si>
-  <si>
-    <t>L1 Sp9D1</t>
-  </si>
-  <si>
-    <t>L1 Sp9D2</t>
-  </si>
-  <si>
-    <t>L2 Sp9D3</t>
-  </si>
-  <si>
-    <t>L3 Sp9D5</t>
-  </si>
-  <si>
-    <t>L4 Sp9D8</t>
-  </si>
-  <si>
-    <t>L5 Sp9D4</t>
-  </si>
-  <si>
-    <t>L6 Sp9D7</t>
-  </si>
-  <si>
-    <t>L6/WM Sp9D9</t>
-  </si>
-  <si>
-    <t>WM Sp9D6</t>
+    <t>L1 Sp07D01</t>
+  </si>
+  <si>
+    <t>L2/3 Sp07D02</t>
+  </si>
+  <si>
+    <t>L3/4 Sp07D03</t>
+  </si>
+  <si>
+    <t>L5 Sp07D04</t>
+  </si>
+  <si>
+    <t>L6 Sp07D06</t>
+  </si>
+  <si>
+    <t>WM Sp07D05</t>
+  </si>
+  <si>
+    <t>WM Sp07D07</t>
+  </si>
+  <si>
+    <t>L1 Sp09D01</t>
+  </si>
+  <si>
+    <t>L1 Sp09D02</t>
+  </si>
+  <si>
+    <t>L2/3 Sp09D03</t>
+  </si>
+  <si>
+    <t>L3 Sp09D05</t>
+  </si>
+  <si>
+    <t>L4 Sp09D08</t>
+  </si>
+  <si>
+    <t>L5 Sp09D04</t>
+  </si>
+  <si>
+    <t>L6 Sp09D07</t>
+  </si>
+  <si>
+    <t>WM Sp09D06</t>
+  </si>
+  <si>
+    <t>WM Sp09D09</t>
   </si>
   <si>
     <t>L1 Sp16D01</t>
@@ -343,12 +343,12 @@
     <t>L2 Sp16D08</t>
   </si>
   <si>
+    <t>L2/3 Sp16D10</t>
+  </si>
+  <si>
     <t>L3 Sp16D03</t>
   </si>
   <si>
-    <t>L3 Sp16D10</t>
-  </si>
-  <si>
     <t>L3/4 Sp16D09</t>
   </si>
   <si>
@@ -367,18 +367,21 @@
     <t>L6 Sp16D12</t>
   </si>
   <si>
-    <t>L6/WM Sp16D13</t>
-  </si>
-  <si>
     <t>WM Sp16D06</t>
   </si>
   <si>
     <t>WM Sp16D11</t>
   </si>
   <si>
+    <t>WM Sp16D13</t>
+  </si>
+  <si>
     <t>WM Sp16D15</t>
   </si>
   <si>
+    <t>L1 Sp28D11</t>
+  </si>
+  <si>
     <t>L1 Sp28D12</t>
   </si>
   <si>
@@ -394,9 +397,6 @@
     <t>L1 Sp28D27</t>
   </si>
   <si>
-    <t>L1/2 Sp28D11</t>
-  </si>
-  <si>
     <t>L2 Sp28D09</t>
   </si>
   <si>
@@ -415,15 +415,15 @@
     <t>L3/4 Sp28D10</t>
   </si>
   <si>
+    <t>L3/4 Sp28D24</t>
+  </si>
+  <si>
     <t>L4 Sp28D05</t>
   </si>
   <si>
     <t>L4 Sp28D22</t>
   </si>
   <si>
-    <t>L4 Sp28D24</t>
-  </si>
-  <si>
     <t>L4 Sp28D25</t>
   </si>
   <si>
@@ -433,15 +433,15 @@
     <t>L5 Sp28D13</t>
   </si>
   <si>
+    <t>L5/6 Sp28D19</t>
+  </si>
+  <si>
     <t>L6 Sp28D07</t>
   </si>
   <si>
     <t>L6 Sp28D14</t>
   </si>
   <si>
-    <t>L6 Sp28D19</t>
-  </si>
-  <si>
     <t>L6/WM Sp28D16</t>
   </si>
   <si>
@@ -457,10 +457,10 @@
     <t>WM Sp28D28</t>
   </si>
   <si>
-    <t>k7</t>
-  </si>
-  <si>
-    <t>k9</t>
+    <t>k07</t>
+  </si>
+  <si>
+    <t>k09</t>
   </si>
   <si>
     <t>k16</t>
@@ -469,52 +469,52 @@
     <t>k28</t>
   </si>
   <si>
-    <t>Sp7D1</t>
-  </si>
-  <si>
-    <t>Sp7D2</t>
-  </si>
-  <si>
-    <t>Sp7D3</t>
-  </si>
-  <si>
-    <t>Sp7D4</t>
-  </si>
-  <si>
-    <t>Sp7D6</t>
-  </si>
-  <si>
-    <t>Sp7D5</t>
-  </si>
-  <si>
-    <t>Sp7D7</t>
-  </si>
-  <si>
-    <t>Sp9D1</t>
-  </si>
-  <si>
-    <t>Sp9D2</t>
-  </si>
-  <si>
-    <t>Sp9D3</t>
-  </si>
-  <si>
-    <t>Sp9D5</t>
-  </si>
-  <si>
-    <t>Sp9D8</t>
-  </si>
-  <si>
-    <t>Sp9D4</t>
-  </si>
-  <si>
-    <t>Sp9D7</t>
-  </si>
-  <si>
-    <t>Sp9D9</t>
-  </si>
-  <si>
-    <t>Sp9D6</t>
+    <t>Sp07D01</t>
+  </si>
+  <si>
+    <t>Sp07D02</t>
+  </si>
+  <si>
+    <t>Sp07D03</t>
+  </si>
+  <si>
+    <t>Sp07D04</t>
+  </si>
+  <si>
+    <t>Sp07D06</t>
+  </si>
+  <si>
+    <t>Sp07D05</t>
+  </si>
+  <si>
+    <t>Sp07D07</t>
+  </si>
+  <si>
+    <t>Sp09D01</t>
+  </si>
+  <si>
+    <t>Sp09D02</t>
+  </si>
+  <si>
+    <t>Sp09D03</t>
+  </si>
+  <si>
+    <t>Sp09D05</t>
+  </si>
+  <si>
+    <t>Sp09D08</t>
+  </si>
+  <si>
+    <t>Sp09D04</t>
+  </si>
+  <si>
+    <t>Sp09D07</t>
+  </si>
+  <si>
+    <t>Sp09D06</t>
+  </si>
+  <si>
+    <t>Sp09D09</t>
   </si>
   <si>
     <t>Sp16D01</t>
@@ -529,12 +529,12 @@
     <t>Sp16D08</t>
   </si>
   <si>
+    <t>Sp16D10</t>
+  </si>
+  <si>
     <t>Sp16D03</t>
   </si>
   <si>
-    <t>Sp16D10</t>
-  </si>
-  <si>
     <t>Sp16D09</t>
   </si>
   <si>
@@ -553,18 +553,21 @@
     <t>Sp16D12</t>
   </si>
   <si>
+    <t>Sp16D06</t>
+  </si>
+  <si>
+    <t>Sp16D11</t>
+  </si>
+  <si>
     <t>Sp16D13</t>
   </si>
   <si>
-    <t>Sp16D06</t>
-  </si>
-  <si>
-    <t>Sp16D11</t>
-  </si>
-  <si>
     <t>Sp16D15</t>
   </si>
   <si>
+    <t>Sp28D11</t>
+  </si>
+  <si>
     <t>Sp28D12</t>
   </si>
   <si>
@@ -580,9 +583,6 @@
     <t>Sp28D27</t>
   </si>
   <si>
-    <t>Sp28D11</t>
-  </si>
-  <si>
     <t>Sp28D09</t>
   </si>
   <si>
@@ -601,15 +601,15 @@
     <t>Sp28D10</t>
   </si>
   <si>
+    <t>Sp28D24</t>
+  </si>
+  <si>
     <t>Sp28D05</t>
   </si>
   <si>
     <t>Sp28D22</t>
   </si>
   <si>
-    <t>Sp28D24</t>
-  </si>
-  <si>
     <t>Sp28D25</t>
   </si>
   <si>
@@ -619,15 +619,15 @@
     <t>Sp28D13</t>
   </si>
   <si>
+    <t>Sp28D19</t>
+  </si>
+  <si>
     <t>Sp28D07</t>
   </si>
   <si>
     <t>Sp28D14</t>
   </si>
   <si>
-    <t>Sp28D19</t>
-  </si>
-  <si>
     <t>Sp28D16</t>
   </si>
   <si>
@@ -649,10 +649,13 @@
     <t>L4/3</t>
   </si>
   <si>
+    <t>L3/2</t>
+  </si>
+  <si>
+    <t>L6/5</t>
+  </si>
+  <si>
     <t>WM/L6</t>
-  </si>
-  <si>
-    <t>L2/1</t>
   </si>
   <si>
     <t>Layer6</t>
@@ -1014,7 +1017,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
         <v>39</v>
@@ -1032,12 +1035,12 @@
         <v>208</v>
       </c>
       <c r="G11" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
         <v>40</v>
@@ -1055,12 +1058,12 @@
         <v>208</v>
       </c>
       <c r="G12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
         <v>41</v>
@@ -1078,7 +1081,7 @@
         <v>208</v>
       </c>
       <c r="G13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14">
@@ -1129,7 +1132,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B16" t="s">
         <v>44</v>
@@ -1147,7 +1150,7 @@
         <v>208</v>
       </c>
       <c r="G16" t="s">
-        <v>210</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17">
@@ -1244,7 +1247,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B21" t="s">
         <v>49</v>
@@ -1262,12 +1265,12 @@
         <v>208</v>
       </c>
       <c r="G21" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
         <v>50</v>
@@ -1285,12 +1288,12 @@
         <v>208</v>
       </c>
       <c r="G22" t="s">
-        <v>26</v>
+        <v>210</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B23" t="s">
         <v>51</v>
@@ -1308,7 +1311,7 @@
         <v>208</v>
       </c>
       <c r="G23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24">
@@ -1336,7 +1339,7 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B25" t="s">
         <v>53</v>
@@ -1354,7 +1357,7 @@
         <v>208</v>
       </c>
       <c r="G25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26">
@@ -1451,7 +1454,7 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B30" t="s">
         <v>58</v>
@@ -1469,7 +1472,7 @@
         <v>208</v>
       </c>
       <c r="G30" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31">
@@ -1658,7 +1661,7 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B39" t="s">
         <v>67</v>
@@ -1676,12 +1679,12 @@
         <v>208</v>
       </c>
       <c r="G39" t="s">
-        <v>211</v>
+        <v>19</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B40" t="s">
         <v>68</v>
@@ -1699,12 +1702,12 @@
         <v>208</v>
       </c>
       <c r="G40" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B41" t="s">
         <v>69</v>
@@ -1722,12 +1725,12 @@
         <v>208</v>
       </c>
       <c r="G41" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B42" t="s">
         <v>70</v>
@@ -1745,12 +1748,12 @@
         <v>208</v>
       </c>
       <c r="G42" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B43" t="s">
         <v>71</v>
@@ -1768,12 +1771,12 @@
         <v>208</v>
       </c>
       <c r="G43" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B44" t="s">
         <v>72</v>
@@ -1791,7 +1794,7 @@
         <v>208</v>
       </c>
       <c r="G44" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="45">
@@ -1819,7 +1822,7 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B46" t="s">
         <v>74</v>
@@ -1837,12 +1840,12 @@
         <v>208</v>
       </c>
       <c r="G46" t="s">
-        <v>27</v>
+        <v>209</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B47" t="s">
         <v>75</v>
@@ -1860,12 +1863,12 @@
         <v>208</v>
       </c>
       <c r="G47" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B48" t="s">
         <v>76</v>
@@ -1883,12 +1886,12 @@
         <v>208</v>
       </c>
       <c r="G48" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B49" t="s">
         <v>77</v>
@@ -1906,7 +1909,7 @@
         <v>208</v>
       </c>
       <c r="G49" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="50">
@@ -1957,7 +1960,7 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B52" t="s">
         <v>80</v>
@@ -1975,7 +1978,7 @@
         <v>208</v>
       </c>
       <c r="G52" t="s">
-        <v>23</v>
+        <v>211</v>
       </c>
     </row>
     <row r="53">
@@ -2026,7 +2029,7 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B55" t="s">
         <v>83</v>
@@ -2044,7 +2047,7 @@
         <v>208</v>
       </c>
       <c r="G55" t="s">
-        <v>28</v>
+        <v>212</v>
       </c>
     </row>
     <row r="56">
@@ -2155,25 +2158,25 @@
     <row r="1">
       <c r="A1"/>
       <c r="B1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F1" t="s">
+        <v>152</v>
+      </c>
+      <c r="G1" t="s">
         <v>153</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" t="s">
         <v>154</v>
-      </c>
-      <c r="D1" t="s">
-        <v>155</v>
-      </c>
-      <c r="E1" t="s">
-        <v>156</v>
-      </c>
-      <c r="F1" t="s">
-        <v>150</v>
-      </c>
-      <c r="G1" t="s">
-        <v>151</v>
-      </c>
-      <c r="H1" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="2">
@@ -2181,181 +2184,181 @@
         <v>24</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.11145753215176998</v>
+        <v>0.08660062969117822</v>
       </c>
       <c r="C2" t="n">
-        <v>0.2544364878068629</v>
+        <v>0.9456898796852619</v>
       </c>
       <c r="D2" t="n">
-        <v>0.8185236691837032</v>
+        <v>0.7857668336202132</v>
       </c>
       <c r="E2" t="n">
-        <v>0.4979517032803125</v>
+        <v>-0.703168222171207</v>
       </c>
       <c r="F2" t="n">
-        <v>0.04991036729106847</v>
+        <v>-0.7304689702950955</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.4979642498667257</v>
+        <v>-0.4405351412196086</v>
       </c>
       <c r="H2" t="n">
-        <v>-0.5895211995152212</v>
+        <v>-0.16357202679915997</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B3" t="n">
-        <v>0.048674391691589</v>
+        <v>-0.4340853700232825</v>
       </c>
       <c r="C3" t="n">
-        <v>0.8380773487308874</v>
+        <v>0.14427111663479428</v>
       </c>
       <c r="D3" t="n">
-        <v>0.43714238759280616</v>
+        <v>0.28065608542914505</v>
       </c>
       <c r="E3" t="n">
-        <v>0.32619210522509795</v>
+        <v>-0.3456118303240812</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.2769618850662076</v>
+        <v>-0.350131745075143</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.5060411746634701</v>
+        <v>0.17716847094818242</v>
       </c>
       <c r="H3" t="n">
-        <v>-0.5296916563870404</v>
+        <v>0.8703054108497322</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B4" t="n">
-        <v>0.8657380901033234</v>
+        <v>-0.5086105497177728</v>
       </c>
       <c r="C4" t="n">
-        <v>0.20217627611630976</v>
+        <v>-0.22259257788519182</v>
       </c>
       <c r="D4" t="n">
-        <v>0.014787195384767403</v>
+        <v>-0.12706790495966055</v>
       </c>
       <c r="E4" t="n">
-        <v>0.009169819750654522</v>
+        <v>-0.28421407307668256</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.4012821576354229</v>
+        <v>0.2309750168074776</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.5132715268275537</v>
+        <v>0.9009592363368231</v>
       </c>
       <c r="H4" t="n">
-        <v>-0.09036405099662512</v>
+        <v>0.3433636015349134</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B5" t="n">
-        <v>0.320964460114364</v>
+        <v>-0.3521447758367443</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.2989899751645608</v>
+        <v>-0.420832961573367</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.29950283058662697</v>
+        <v>-0.4574811494505126</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.23924422304095194</v>
+        <v>0.11556203304777851</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.2417743141089688</v>
+        <v>0.8088068215916977</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.050003227771032714</v>
+        <v>0.5758024008267725</v>
       </c>
       <c r="H5" t="n">
-        <v>0.6869694431415555</v>
+        <v>-0.11240526294299671</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.3581898693016773</v>
+        <v>-0.010171671637480926</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.4976871330157516</v>
+        <v>-0.6588935627231943</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.5155980318092483</v>
+        <v>-0.6533933751430407</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.2828168799742204</v>
+        <v>0.8317515738333782</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.010559318883535361</v>
+        <v>0.7488153111236104</v>
       </c>
       <c r="G6" t="n">
-        <v>0.7162676443730147</v>
+        <v>-0.025509865767148365</v>
       </c>
       <c r="H6" t="n">
-        <v>0.655152186179755</v>
+        <v>-0.23060036504821907</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.4838986773235351</v>
+        <v>0.15585493201312609</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.34257943155597337</v>
+        <v>-0.46911493039457136</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.38372711328358733</v>
+        <v>-0.41956421431437546</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.2503277060918604</v>
+        <v>0.841837149022825</v>
       </c>
       <c r="F7" t="n">
-        <v>0.21640944747933513</v>
+        <v>0.18980459237037614</v>
       </c>
       <c r="G7" t="n">
-        <v>0.8405874123454564</v>
+        <v>-0.2927599907305512</v>
       </c>
       <c r="H7" t="n">
-        <v>0.10721226088559252</v>
+        <v>-0.06348084812420124</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.4396034051162523</v>
+        <v>0.9093240054734891</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.39428423566721715</v>
+        <v>-0.03136033444546572</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.1394001317890834</v>
+        <v>-0.024815451015961963</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.1294170869210736</v>
+        <v>0.1325671450562423</v>
       </c>
       <c r="F8" t="n">
-        <v>0.8647959657342402</v>
+        <v>-0.2681293810616702</v>
       </c>
       <c r="G8" t="n">
-        <v>0.20233030954355039</v>
+        <v>-0.545656476613206</v>
       </c>
       <c r="H8" t="n">
-        <v>-0.17644920516981855</v>
+        <v>-0.5413264400619362</v>
       </c>
     </row>
   </sheetData>
@@ -2380,22 +2383,22 @@
         <v>158</v>
       </c>
       <c r="D1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E1" t="s">
+        <v>165</v>
+      </c>
+      <c r="F1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G1" t="s">
+        <v>163</v>
+      </c>
+      <c r="H1" t="s">
         <v>159</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>160</v>
-      </c>
-      <c r="F1" t="s">
-        <v>163</v>
-      </c>
-      <c r="G1" t="s">
-        <v>165</v>
-      </c>
-      <c r="H1" t="s">
-        <v>164</v>
-      </c>
-      <c r="I1" t="s">
-        <v>162</v>
       </c>
       <c r="J1" t="s">
         <v>161</v>
@@ -2406,223 +2409,223 @@
         <v>24</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.10654859275961132</v>
+        <v>0.18233409248506321</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.0035433413464811296</v>
+        <v>0.10116109321566395</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.4235366207200138</v>
+        <v>0.9452202433345341</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.5476204707928011</v>
+        <v>0.8038452401893256</v>
       </c>
       <c r="F2" t="n">
-        <v>0.20277526117099703</v>
+        <v>-0.3756919512330929</v>
       </c>
       <c r="G2" t="n">
-        <v>0.8491811536784114</v>
+        <v>-0.1819621162663477</v>
       </c>
       <c r="H2" t="n">
-        <v>0.7460555093739256</v>
+        <v>-0.6340380051280985</v>
       </c>
       <c r="I2" t="n">
-        <v>-0.07587410324851152</v>
+        <v>-0.7940434813686468</v>
       </c>
       <c r="J2" t="n">
-        <v>-0.4453557665329263</v>
+        <v>-0.6286441496949572</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.15972132432106445</v>
+        <v>-0.28515927125845497</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.24997282472767376</v>
+        <v>-0.3742808103087616</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.4150160360045598</v>
+        <v>0.13145478640958205</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.5243084930240072</v>
+        <v>0.5302265400880759</v>
       </c>
       <c r="F3" t="n">
-        <v>0.8357292105745026</v>
+        <v>0.2503070267569068</v>
       </c>
       <c r="G3" t="n">
-        <v>0.3187643852112042</v>
+        <v>0.8631575902918986</v>
       </c>
       <c r="H3" t="n">
-        <v>0.6422798056870652</v>
+        <v>-0.267699954622677</v>
       </c>
       <c r="I3" t="n">
-        <v>0.10193211993069361</v>
+        <v>-0.33654306413292895</v>
       </c>
       <c r="J3" t="n">
-        <v>-0.44933444253970234</v>
+        <v>-0.22786700724759576</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.2168999123307011</v>
+        <v>-0.34484934977670956</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.35122879845987476</v>
+        <v>-0.4862492001819124</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.4661136640871984</v>
+        <v>-0.19214050745655667</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.2703070067587606</v>
+        <v>-0.04815214362516406</v>
       </c>
       <c r="F4" t="n">
-        <v>0.22739107870819167</v>
+        <v>0.9257536491525145</v>
       </c>
       <c r="G4" t="n">
-        <v>0.020038546138316564</v>
+        <v>0.4172568716280277</v>
       </c>
       <c r="H4" t="n">
-        <v>0.008250033613566281</v>
+        <v>-0.30703556687043404</v>
       </c>
       <c r="I4" t="n">
-        <v>0.8714146161686624</v>
+        <v>0.04368405258338519</v>
       </c>
       <c r="J4" t="n">
-        <v>0.11458354600539764</v>
+        <v>0.38992075891358086</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.13020233670858566</v>
+        <v>-0.28101291175617527</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.2508434323323941</v>
+        <v>-0.3986331047681389</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.11920022540949334</v>
+        <v>-0.3962732830634432</v>
       </c>
       <c r="E5" t="n">
-        <v>0.37230394871617783</v>
+        <v>-0.5272924111084012</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.2761243076858473</v>
+        <v>0.5492681141632048</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.29370854758061693</v>
+        <v>-0.03938880566569008</v>
       </c>
       <c r="H5" t="n">
-        <v>-0.4053801829231407</v>
+        <v>0.002362978231716639</v>
       </c>
       <c r="I5" t="n">
-        <v>0.28084201495520855</v>
+        <v>0.5692207638043618</v>
       </c>
       <c r="J5" t="n">
-        <v>0.7861311489117287</v>
+        <v>0.886617952543041</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B6" t="n">
-        <v>0.09113952690535314</v>
+        <v>-0.11403512224647375</v>
       </c>
       <c r="C6" t="n">
-        <v>0.014467091391145272</v>
+        <v>-0.06103860756914444</v>
       </c>
       <c r="D6" t="n">
-        <v>0.6144496151190173</v>
+        <v>-0.665129523126223</v>
       </c>
       <c r="E6" t="n">
-        <v>0.7770769685009092</v>
+        <v>-0.7583633314635398</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.5113683367861849</v>
+        <v>-0.08857852853631731</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.50517100746603</v>
+        <v>-0.23049140606647356</v>
       </c>
       <c r="H6" t="n">
-        <v>-0.5993188247596106</v>
+        <v>0.7563890580955026</v>
       </c>
       <c r="I6" t="n">
-        <v>-0.3964394183835748</v>
+        <v>0.8972083564188468</v>
       </c>
       <c r="J6" t="n">
-        <v>0.45385709278839087</v>
+        <v>0.5874068204253086</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B7" t="n">
-        <v>0.07523732569181367</v>
+        <v>-0.0454523774864195</v>
       </c>
       <c r="C7" t="n">
-        <v>0.23825494305523287</v>
+        <v>0.17502466270998837</v>
       </c>
       <c r="D7" t="n">
-        <v>0.865105283385567</v>
+        <v>-0.48744631958558693</v>
       </c>
       <c r="E7" t="n">
-        <v>0.44938551458178266</v>
+        <v>-0.42804452746699106</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.3314018851283685</v>
+        <v>-0.32876891000139147</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.40142786608643305</v>
+        <v>-0.09099482789754662</v>
       </c>
       <c r="H7" t="n">
-        <v>-0.36843715982801817</v>
+        <v>0.8922991320258268</v>
       </c>
       <c r="I7" t="n">
-        <v>-0.47600825653913614</v>
+        <v>0.49706489375206103</v>
       </c>
       <c r="J7" t="n">
-        <v>-0.08859084307963899</v>
+        <v>-0.0061334148746578585</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B8" t="n">
-        <v>0.5633465430589106</v>
+        <v>0.6747530442684894</v>
       </c>
       <c r="C8" t="n">
-        <v>0.7896539906814056</v>
+        <v>0.8700732349717306</v>
       </c>
       <c r="D8" t="n">
-        <v>0.1997986418339004</v>
+        <v>-0.047160066578838145</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.06475515663438926</v>
+        <v>-0.20522960157831152</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.413005005012456</v>
+        <v>-0.6114803315484088</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.15238428426114908</v>
+        <v>-0.6035094347578965</v>
       </c>
       <c r="H8" t="n">
-        <v>-0.28469835309787306</v>
+        <v>0.08707286710222814</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.47467791958369954</v>
+        <v>-0.19646796554293255</v>
       </c>
       <c r="J8" t="n">
-        <v>-0.29939241118072385</v>
+        <v>-0.43881914191839133</v>
       </c>
     </row>
   </sheetData>
@@ -2641,37 +2644,37 @@
     <row r="1">
       <c r="A1"/>
       <c r="B1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E1" t="s">
         <v>178</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
+        <v>181</v>
+      </c>
+      <c r="G1" t="s">
+        <v>179</v>
+      </c>
+      <c r="H1" t="s">
         <v>180</v>
       </c>
-      <c r="D1" t="s">
-        <v>179</v>
-      </c>
-      <c r="E1" t="s">
-        <v>181</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>174</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>175</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>176</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>177</v>
-      </c>
-      <c r="J1" t="s">
-        <v>167</v>
-      </c>
-      <c r="K1" t="s">
-        <v>166</v>
-      </c>
-      <c r="L1" t="s">
-        <v>168</v>
       </c>
       <c r="M1" t="s">
         <v>173</v>
@@ -2680,13 +2683,13 @@
         <v>172</v>
       </c>
       <c r="O1" t="s">
+        <v>171</v>
+      </c>
+      <c r="P1" t="s">
         <v>169</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>170</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="2">
@@ -2694,370 +2697,370 @@
         <v>24</v>
       </c>
       <c r="B2" t="n">
-        <v>0.653901796033738</v>
+        <v>0.10623370693351285</v>
       </c>
       <c r="C2" t="n">
-        <v>0.6523521314708299</v>
+        <v>-0.08267214344632225</v>
       </c>
       <c r="D2" t="n">
-        <v>0.8844820053911119</v>
+        <v>0.13769859508135188</v>
       </c>
       <c r="E2" t="n">
-        <v>0.900114757775504</v>
+        <v>0.9324690598162875</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.2673025968230917</v>
+        <v>0.9376035235564886</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.23799554639708953</v>
+        <v>0.7612907705281787</v>
       </c>
       <c r="H2" t="n">
-        <v>-0.022244132956924418</v>
+        <v>0.7078324597805657</v>
       </c>
       <c r="I2" t="n">
-        <v>0.06773182878899804</v>
+        <v>-0.46304116555464747</v>
       </c>
       <c r="J2" t="n">
-        <v>-0.12252546399255004</v>
+        <v>-0.4293173486036175</v>
       </c>
       <c r="K2" t="n">
-        <v>-0.031479917984331966</v>
+        <v>-0.3069206290113158</v>
       </c>
       <c r="L2" t="n">
-        <v>0.08902885524916838</v>
+        <v>-0.07529462489672085</v>
       </c>
       <c r="M2" t="n">
-        <v>-0.5830338232844454</v>
+        <v>-0.6739087409765425</v>
       </c>
       <c r="N2" t="n">
-        <v>-0.6613420396913755</v>
+        <v>-0.725204189539131</v>
       </c>
       <c r="O2" t="n">
-        <v>-0.5414814971957709</v>
+        <v>-0.812447350558036</v>
       </c>
       <c r="P2" t="n">
-        <v>-0.6582792252148434</v>
+        <v>-0.6719594424325679</v>
       </c>
       <c r="Q2" t="n">
-        <v>-0.6015541000581642</v>
+        <v>-0.5744331439226147</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B3" t="n">
-        <v>0.6731650793281749</v>
+        <v>-0.2837111938160821</v>
       </c>
       <c r="C3" t="n">
-        <v>0.34979827998784857</v>
+        <v>-0.392003544371284</v>
       </c>
       <c r="D3" t="n">
-        <v>0.133676862314046</v>
+        <v>-0.38218522595491855</v>
       </c>
       <c r="E3" t="n">
-        <v>0.32551346913287327</v>
+        <v>0.03986185832164309</v>
       </c>
       <c r="F3" t="n">
-        <v>0.1579605576512254</v>
+        <v>0.19095028805064332</v>
       </c>
       <c r="G3" t="n">
-        <v>0.07702142108832073</v>
+        <v>0.32182396105397765</v>
       </c>
       <c r="H3" t="n">
-        <v>0.8147549324463221</v>
+        <v>0.6057401648062378</v>
       </c>
       <c r="I3" t="n">
-        <v>0.6104864370646971</v>
+        <v>0.2846453282564251</v>
       </c>
       <c r="J3" t="n">
-        <v>-0.28662527549414646</v>
+        <v>0.17321455585679027</v>
       </c>
       <c r="K3" t="n">
-        <v>-0.20827055908542003</v>
+        <v>0.8162905523842747</v>
       </c>
       <c r="L3" t="n">
-        <v>-0.3004105831534908</v>
+        <v>0.617942524720362</v>
       </c>
       <c r="M3" t="n">
-        <v>-0.4194776064824842</v>
+        <v>-0.2396867952985173</v>
       </c>
       <c r="N3" t="n">
-        <v>-0.3881465753213264</v>
+        <v>-0.19753879859134477</v>
       </c>
       <c r="O3" t="n">
-        <v>-0.3871830171225574</v>
+        <v>-0.32937848397777025</v>
       </c>
       <c r="P3" t="n">
-        <v>-0.49243414970030647</v>
+        <v>-0.23322485774539362</v>
       </c>
       <c r="Q3" t="n">
-        <v>-0.3100558496297737</v>
+        <v>-0.24994909738262677</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B4" t="n">
-        <v>0.018472530236101733</v>
+        <v>-0.32280653004805304</v>
       </c>
       <c r="C4" t="n">
-        <v>0.00903034118323909</v>
+        <v>-0.47502254054936754</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.1406852962513169</v>
+        <v>-0.5084873185555933</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.10538722753477121</v>
+        <v>-0.2733598559532801</v>
       </c>
       <c r="F4" t="n">
-        <v>0.8521174837339025</v>
+        <v>-0.20314592099261913</v>
       </c>
       <c r="G4" t="n">
-        <v>0.8179384317228323</v>
+        <v>-0.07545417958075823</v>
       </c>
       <c r="H4" t="n">
-        <v>0.21735465999025563</v>
+        <v>0.014923159118625406</v>
       </c>
       <c r="I4" t="n">
-        <v>0.39630205478129604</v>
+        <v>0.8874504552207647</v>
       </c>
       <c r="J4" t="n">
-        <v>-0.4393909509006497</v>
+        <v>0.8698882418309373</v>
       </c>
       <c r="K4" t="n">
-        <v>-0.24691119301446202</v>
+        <v>0.39056696759828224</v>
       </c>
       <c r="L4" t="n">
-        <v>-0.39220799304126586</v>
+        <v>0.5053578630351848</v>
       </c>
       <c r="M4" t="n">
-        <v>0.11994265890263138</v>
+        <v>0.35631939341537733</v>
       </c>
       <c r="N4" t="n">
-        <v>0.12040318469822756</v>
+        <v>0.30409683145337446</v>
       </c>
       <c r="O4" t="n">
-        <v>-0.38865361984740643</v>
+        <v>-0.003941282239027194</v>
       </c>
       <c r="P4" t="n">
-        <v>-0.23025682946296783</v>
+        <v>-0.25896577305422697</v>
       </c>
       <c r="Q4" t="n">
-        <v>-0.06938606881415621</v>
+        <v>-0.08902828657016719</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.4166434132180585</v>
+        <v>-0.2454755697579533</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.3377142034402647</v>
+        <v>-0.3473049878491409</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.33192163429334876</v>
+        <v>-0.38873652749128407</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.40514903151010384</v>
+        <v>-0.3979726995545743</v>
       </c>
       <c r="F5" t="n">
-        <v>0.33312243887851184</v>
+        <v>-0.4649964571489065</v>
       </c>
       <c r="G5" t="n">
-        <v>0.47319727052338806</v>
+        <v>-0.4054796399824032</v>
       </c>
       <c r="H5" t="n">
-        <v>-0.22516216542636688</v>
+        <v>-0.47883394208385666</v>
       </c>
       <c r="I5" t="n">
-        <v>-0.0510022513537472</v>
+        <v>0.5316789386151662</v>
       </c>
       <c r="J5" t="n">
-        <v>-0.2927590497760535</v>
+        <v>0.6218039149229553</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.15418264812964894</v>
+        <v>-0.025760252710276422</v>
       </c>
       <c r="L5" t="n">
-        <v>-0.28211293866482345</v>
+        <v>0.04411911782137132</v>
       </c>
       <c r="M5" t="n">
-        <v>0.7700880448672098</v>
+        <v>0.8560078210346629</v>
       </c>
       <c r="N5" t="n">
-        <v>0.7093930487009983</v>
+        <v>0.7693205632963193</v>
       </c>
       <c r="O5" t="n">
-        <v>-0.002165362998576565</v>
+        <v>0.5034141524562444</v>
       </c>
       <c r="P5" t="n">
-        <v>0.3885529304261185</v>
+        <v>0.04985451502705304</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.17659402983884256</v>
+        <v>0.17256725714162546</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.6804581614791811</v>
+        <v>-0.05692450410370169</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.47938379621330246</v>
+        <v>0.0912562227471629</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.5047186772775014</v>
+        <v>-0.06694183136595373</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.6415058672928396</v>
+        <v>-0.6202345203562702</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.22007777870763343</v>
+        <v>-0.7032023237585672</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.20492951375533527</v>
+        <v>-0.662160496752198</v>
       </c>
       <c r="H6" t="n">
-        <v>-0.37113694909676764</v>
+        <v>-0.7180562095435445</v>
       </c>
       <c r="I6" t="n">
-        <v>-0.4096673521285494</v>
+        <v>0.011546289844407087</v>
       </c>
       <c r="J6" t="n">
-        <v>0.13282966830367887</v>
+        <v>0.020808856047984943</v>
       </c>
       <c r="K6" t="n">
-        <v>0.048574483365911754</v>
+        <v>-0.09125144941524208</v>
       </c>
       <c r="L6" t="n">
-        <v>0.021227536776471805</v>
+        <v>-0.3079482774220605</v>
       </c>
       <c r="M6" t="n">
-        <v>0.5901317274422414</v>
+        <v>0.6428869899018458</v>
       </c>
       <c r="N6" t="n">
-        <v>0.6612837801126555</v>
+        <v>0.7143680188331257</v>
       </c>
       <c r="O6" t="n">
-        <v>0.6959458862802437</v>
+        <v>0.9071869801247692</v>
       </c>
       <c r="P6" t="n">
-        <v>0.8436012737073166</v>
+        <v>0.7665889315973625</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.5562290439387911</v>
+        <v>0.5767535452249377</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.3849819475006454</v>
+        <v>-0.012669879332764705</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.3657274005702816</v>
+        <v>0.3343551553266733</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.405158991991442</v>
+        <v>0.11608998739760935</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.4317146001525615</v>
+        <v>-0.45811679550048345</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.34571248098665297</v>
+        <v>-0.46552388187428834</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.3943486009672154</v>
+        <v>-0.4391615973711572</v>
       </c>
       <c r="H7" t="n">
-        <v>-0.16326239037543344</v>
+        <v>-0.3996949336958158</v>
       </c>
       <c r="I7" t="n">
-        <v>-0.38030778900068024</v>
+        <v>-0.2161283646737019</v>
       </c>
       <c r="J7" t="n">
-        <v>0.430846506366691</v>
+        <v>-0.27441360724677644</v>
       </c>
       <c r="K7" t="n">
-        <v>0.04902724341464856</v>
+        <v>0.04760049836177583</v>
       </c>
       <c r="L7" t="n">
-        <v>0.13884011644783673</v>
+        <v>-0.30177258344158875</v>
       </c>
       <c r="M7" t="n">
-        <v>0.0985351237509444</v>
+        <v>0.07507506882881715</v>
       </c>
       <c r="N7" t="n">
-        <v>0.18381075579021766</v>
+        <v>0.21811990018049413</v>
       </c>
       <c r="O7" t="n">
-        <v>0.8537486069382917</v>
+        <v>0.5667940580925148</v>
       </c>
       <c r="P7" t="n">
-        <v>0.5577719088152455</v>
+        <v>0.8704932383190563</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.44383885380102694</v>
+        <v>0.5462517820242165</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.29992569488808307</v>
+        <v>0.6334779047728258</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.19641283947079435</v>
+        <v>0.8290645755848722</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.03450547050798898</v>
+        <v>0.8603122764633632</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.09201114857628119</v>
+        <v>0.02729586958707751</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.48912694784657423</v>
+        <v>-0.04720643394696053</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.5059318060780609</v>
+        <v>-0.11343473555200607</v>
       </c>
       <c r="H8" t="n">
-        <v>-0.4135729333498962</v>
+        <v>-0.30012264635252617</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.4097023183830863</v>
+        <v>-0.6150903434122268</v>
       </c>
       <c r="J8" t="n">
-        <v>0.7339783461653612</v>
+        <v>-0.5831781917405922</v>
       </c>
       <c r="K8" t="n">
-        <v>0.6339278986781055</v>
+        <v>-0.5602218946720319</v>
       </c>
       <c r="L8" t="n">
-        <v>0.7806549277236959</v>
+        <v>-0.4096405727627279</v>
       </c>
       <c r="M8" t="n">
-        <v>-0.25664142069614126</v>
+        <v>-0.3918964107958459</v>
       </c>
       <c r="N8" t="n">
-        <v>-0.2801498462254277</v>
+        <v>-0.4109668296023477</v>
       </c>
       <c r="O8" t="n">
-        <v>0.11899982547024843</v>
+        <v>-0.11197886986841137</v>
       </c>
       <c r="P8" t="n">
-        <v>-0.011635829790945885</v>
+        <v>0.0633208427593049</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.13079530459361177</v>
+        <v>0.10095846102517224</v>
       </c>
     </row>
   </sheetData>
@@ -3097,61 +3100,61 @@
         <v>199</v>
       </c>
       <c r="I1" t="s">
+        <v>200</v>
+      </c>
+      <c r="J1" t="s">
+        <v>201</v>
+      </c>
+      <c r="K1" t="s">
         <v>202</v>
       </c>
-      <c r="J1" t="s">
-        <v>200</v>
-      </c>
-      <c r="K1" t="s">
-        <v>201</v>
-      </c>
       <c r="L1" t="s">
+        <v>182</v>
+      </c>
+      <c r="M1" t="s">
+        <v>186</v>
+      </c>
+      <c r="N1" t="s">
         <v>187</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>185</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q1" t="s">
         <v>184</v>
       </c>
-      <c r="O1" t="s">
-        <v>186</v>
-      </c>
-      <c r="P1" t="s">
-        <v>182</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>183</v>
-      </c>
       <c r="R1" t="s">
+        <v>196</v>
+      </c>
+      <c r="S1" t="s">
+        <v>197</v>
+      </c>
+      <c r="T1" t="s">
+        <v>195</v>
+      </c>
+      <c r="U1" t="s">
+        <v>193</v>
+      </c>
+      <c r="V1" t="s">
+        <v>194</v>
+      </c>
+      <c r="W1" t="s">
+        <v>192</v>
+      </c>
+      <c r="X1" t="s">
         <v>188</v>
       </c>
-      <c r="S1" t="s">
+      <c r="Y1" t="s">
+        <v>189</v>
+      </c>
+      <c r="Z1" t="s">
         <v>190</v>
       </c>
-      <c r="T1" t="s">
+      <c r="AA1" t="s">
         <v>191</v>
-      </c>
-      <c r="U1" t="s">
-        <v>189</v>
-      </c>
-      <c r="V1" t="s">
-        <v>192</v>
-      </c>
-      <c r="W1" t="s">
-        <v>195</v>
-      </c>
-      <c r="X1" t="s">
-        <v>194</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>193</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>196</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="2">
@@ -3159,580 +3162,580 @@
         <v>24</v>
       </c>
       <c r="B2" t="n">
-        <v>0.6493170238396533</v>
+        <v>0.6785571557691567</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9178669220338662</v>
+        <v>0.9308853320227131</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9123599696061124</v>
+        <v>0.9414395270069378</v>
       </c>
       <c r="E2" t="n">
-        <v>0.8903487460014028</v>
+        <v>0.9148347025674697</v>
       </c>
       <c r="F2" t="n">
-        <v>0.7335210989471184</v>
+        <v>0.7583241989245084</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.2500804546810205</v>
+        <v>-0.35316891983583687</v>
       </c>
       <c r="H2" t="n">
-        <v>-0.20404323093176477</v>
+        <v>-0.31576500993927664</v>
       </c>
       <c r="I2" t="n">
-        <v>0.21600336156450442</v>
+        <v>0.1710332869643344</v>
       </c>
       <c r="J2" t="n">
-        <v>-0.09095713946520259</v>
+        <v>-0.2830539601147023</v>
       </c>
       <c r="K2" t="n">
-        <v>0.019620173111368825</v>
+        <v>-0.17720210606110554</v>
       </c>
       <c r="L2" t="n">
-        <v>-0.3095092150153524</v>
+        <v>-0.28607905453023796</v>
       </c>
       <c r="M2" t="n">
-        <v>-0.10030219061261766</v>
+        <v>-0.09786803704097534</v>
       </c>
       <c r="N2" t="n">
-        <v>0.04635394511887894</v>
+        <v>0.1955840761325266</v>
       </c>
       <c r="O2" t="n">
-        <v>0.05855516654827976</v>
+        <v>0.23560667648601483</v>
       </c>
       <c r="P2" t="n">
-        <v>0.044280979058761626</v>
+        <v>0.1495611665802948</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.19607670387785198</v>
+        <v>0.24118550455201282</v>
       </c>
       <c r="R2" t="n">
-        <v>-0.5076008875837874</v>
+        <v>-0.5169398156117935</v>
       </c>
       <c r="S2" t="n">
-        <v>-0.6790314089335541</v>
+        <v>-0.556395941481607</v>
       </c>
       <c r="T2" t="n">
-        <v>-0.6399825476646545</v>
+        <v>-0.6493224464465686</v>
       </c>
       <c r="U2" t="n">
-        <v>-0.5143271528676288</v>
+        <v>-0.6933155707104006</v>
       </c>
       <c r="V2" t="n">
-        <v>-0.4470048364236997</v>
+        <v>-0.6867643705445399</v>
       </c>
       <c r="W2" t="n">
-        <v>-0.43204586753574853</v>
+        <v>-0.5266366221653561</v>
       </c>
       <c r="X2" t="n">
-        <v>-0.563683442321183</v>
+        <v>-0.5832361806082114</v>
       </c>
       <c r="Y2" t="n">
-        <v>-0.6400650222919892</v>
+        <v>-0.5545752031171708</v>
       </c>
       <c r="Z2" t="n">
-        <v>-0.6213321442663894</v>
+        <v>-0.7391877172336278</v>
       </c>
       <c r="AA2" t="n">
-        <v>-0.5150002691453903</v>
+        <v>-0.7708857472968998</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B3" t="n">
-        <v>0.6886512465905202</v>
+        <v>0.6493644804771322</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2319600252907177</v>
+        <v>0.15320948550185776</v>
       </c>
       <c r="D3" t="n">
-        <v>0.14583216008568695</v>
+        <v>0.05839442827036169</v>
       </c>
       <c r="E3" t="n">
-        <v>0.37272523950678216</v>
+        <v>0.3000016872467613</v>
       </c>
       <c r="F3" t="n">
-        <v>0.39744991737925817</v>
+        <v>0.3789778121763037</v>
       </c>
       <c r="G3" t="n">
-        <v>0.22799015750343177</v>
+        <v>0.3639033937652387</v>
       </c>
       <c r="H3" t="n">
-        <v>0.11884849947454931</v>
+        <v>0.23646714969960198</v>
       </c>
       <c r="I3" t="n">
-        <v>0.5744245128666207</v>
+        <v>0.5664872685258029</v>
       </c>
       <c r="J3" t="n">
-        <v>0.68974735747243</v>
+        <v>0.7173524474892737</v>
       </c>
       <c r="K3" t="n">
-        <v>0.8426179268467643</v>
+        <v>0.8574842286565132</v>
       </c>
       <c r="L3" t="n">
-        <v>-0.39434900229870484</v>
+        <v>-0.4032608573229967</v>
       </c>
       <c r="M3" t="n">
-        <v>-0.36069276561926283</v>
+        <v>-0.4086913963026022</v>
       </c>
       <c r="N3" t="n">
-        <v>-0.24720763570405369</v>
+        <v>-0.21667377439452032</v>
       </c>
       <c r="O3" t="n">
-        <v>-0.1519485614584082</v>
+        <v>-0.3089357104210058</v>
       </c>
       <c r="P3" t="n">
-        <v>-0.2500155415525478</v>
+        <v>-0.3449336942670261</v>
       </c>
       <c r="Q3" t="n">
-        <v>-0.23861905613346857</v>
+        <v>-0.32833920883166406</v>
       </c>
       <c r="R3" t="n">
-        <v>-0.3297537734685395</v>
+        <v>-0.029041535624152483</v>
       </c>
       <c r="S3" t="n">
-        <v>-0.3141559925556888</v>
+        <v>-0.07477838003394502</v>
       </c>
       <c r="T3" t="n">
-        <v>-0.4279860708639853</v>
+        <v>-0.26403651979781906</v>
       </c>
       <c r="U3" t="n">
-        <v>-0.19251245790693125</v>
+        <v>-0.14803822555113394</v>
       </c>
       <c r="V3" t="n">
-        <v>-0.26672938049811706</v>
+        <v>-0.06861060450944746</v>
       </c>
       <c r="W3" t="n">
-        <v>-0.08255205113625863</v>
+        <v>-0.2935461144516825</v>
       </c>
       <c r="X3" t="n">
-        <v>-0.3820642204638678</v>
+        <v>-0.21475107628084453</v>
       </c>
       <c r="Y3" t="n">
-        <v>-0.3013670059111281</v>
+        <v>-0.12204019892516499</v>
       </c>
       <c r="Z3" t="n">
-        <v>-0.20311929550899507</v>
+        <v>-0.12485499659463942</v>
       </c>
       <c r="AA3" t="n">
-        <v>-0.21438915834573147</v>
+        <v>-0.3272024367223186</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B4" t="n">
-        <v>0.012879428083367823</v>
+        <v>0.03997820409239257</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.1647845673305864</v>
+        <v>-0.22963826997163414</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.16599698895237472</v>
+        <v>-0.27053730080935007</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.09611568087232958</v>
+        <v>-0.1370505355444134</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.0268883922499935</v>
+        <v>-0.05456774917903086</v>
       </c>
       <c r="G4" t="n">
-        <v>0.8745589345953261</v>
+        <v>0.9013878747870213</v>
       </c>
       <c r="H4" t="n">
-        <v>0.8444393605193122</v>
+        <v>0.8838801885169368</v>
       </c>
       <c r="I4" t="n">
-        <v>0.4983399215151283</v>
+        <v>0.5645274465398896</v>
       </c>
       <c r="J4" t="n">
-        <v>0.4874187699160136</v>
+        <v>0.5864852700220416</v>
       </c>
       <c r="K4" t="n">
-        <v>0.22694474128432454</v>
+        <v>0.36974155715477147</v>
       </c>
       <c r="L4" t="n">
-        <v>-0.43205927564964414</v>
+        <v>-0.4599688211264407</v>
       </c>
       <c r="M4" t="n">
-        <v>-0.4204751208170363</v>
+        <v>-0.46137702353793913</v>
       </c>
       <c r="N4" t="n">
-        <v>-0.28263762073047927</v>
+        <v>-0.31666216921426826</v>
       </c>
       <c r="O4" t="n">
-        <v>-0.2508808781118038</v>
+        <v>-0.4367118292443404</v>
       </c>
       <c r="P4" t="n">
-        <v>-0.3771732679872777</v>
+        <v>-0.5072207844476196</v>
       </c>
       <c r="Q4" t="n">
-        <v>-0.4549914542903667</v>
+        <v>-0.5324821947883036</v>
       </c>
       <c r="R4" t="n">
-        <v>-0.3990824247755686</v>
+        <v>0.5461378072398999</v>
       </c>
       <c r="S4" t="n">
-        <v>-0.12463934523375621</v>
+        <v>0.44024697393021694</v>
       </c>
       <c r="T4" t="n">
-        <v>-0.20772493521083582</v>
+        <v>0.3350137820274316</v>
       </c>
       <c r="U4" t="n">
-        <v>0.03438006883096656</v>
+        <v>0.30076406007064044</v>
       </c>
       <c r="V4" t="n">
-        <v>0.0026832567078510935</v>
+        <v>0.3616359052378082</v>
       </c>
       <c r="W4" t="n">
-        <v>0.4678035910352105</v>
+        <v>0.0035311960662241237</v>
       </c>
       <c r="X4" t="n">
-        <v>0.1463541383788132</v>
+        <v>-0.32516202776627884</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.13731385510401944</v>
+        <v>0.045071630906456675</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.2518755363321562</v>
+        <v>0.006107611185465751</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.30340650727930263</v>
+        <v>-0.0410185270725628</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.46568227909381477</v>
+        <v>-0.5145619859890052</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.42362326261313443</v>
+        <v>-0.48564526335360364</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.35894813340918164</v>
+        <v>-0.42613285492860437</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.41280299574484</v>
+        <v>-0.4701669192556911</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.39489869386695825</v>
+        <v>-0.45175520162462285</v>
       </c>
       <c r="G5" t="n">
-        <v>0.31453278697105297</v>
+        <v>0.4548212349107807</v>
       </c>
       <c r="H5" t="n">
-        <v>0.4505548007388841</v>
+        <v>0.5729893740640809</v>
       </c>
       <c r="I5" t="n">
-        <v>2.2716446379069432E-4</v>
+        <v>0.10257542313924137</v>
       </c>
       <c r="J5" t="n">
-        <v>0.0020097165859310367</v>
+        <v>0.1587349851699436</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.2480687977426747</v>
+        <v>-0.10618774838250228</v>
       </c>
       <c r="L5" t="n">
-        <v>-0.17620604537984264</v>
+        <v>-0.24838095009136088</v>
       </c>
       <c r="M5" t="n">
-        <v>-0.2877606494062909</v>
+        <v>-0.3246028388308533</v>
       </c>
       <c r="N5" t="n">
-        <v>-0.248537887609699</v>
+        <v>-0.30451365523569723</v>
       </c>
       <c r="O5" t="n">
-        <v>-0.21324354023582834</v>
+        <v>-0.39736639338909924</v>
       </c>
       <c r="P5" t="n">
-        <v>-0.3237899682512554</v>
+        <v>-0.42638263314831026</v>
       </c>
       <c r="Q5" t="n">
-        <v>-0.4212430012661145</v>
+        <v>-0.4922569164895986</v>
       </c>
       <c r="R5" t="n">
-        <v>-0.07597180138887903</v>
+        <v>0.7090745811858689</v>
       </c>
       <c r="S5" t="n">
-        <v>0.31747497986825013</v>
+        <v>0.8096979758080329</v>
       </c>
       <c r="T5" t="n">
-        <v>0.3514658970054495</v>
+        <v>0.8420973066011205</v>
       </c>
       <c r="U5" t="n">
-        <v>0.20154305337839296</v>
+        <v>0.7374437818763301</v>
       </c>
       <c r="V5" t="n">
-        <v>0.3054429237591012</v>
+        <v>0.6699833492371541</v>
       </c>
       <c r="W5" t="n">
-        <v>0.579786308691703</v>
+        <v>0.30258506911123834</v>
       </c>
       <c r="X5" t="n">
-        <v>0.7263050997602427</v>
+        <v>-0.061557676785742234</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.6880534053445622</v>
+        <v>0.254083961443421</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.6090119745622712</v>
+        <v>0.34811688627900417</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.7410771034688896</v>
+        <v>0.4491946917539776</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.7096597084734985</v>
+        <v>-0.7232019793467943</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.6337458998976865</v>
+        <v>-0.6868596134566451</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.5641283730275005</v>
+        <v>-0.6437731332321137</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.687382401028845</v>
+        <v>-0.7471362725632142</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.5877011063488875</v>
+        <v>-0.6912243094374262</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.23216849639568976</v>
+        <v>-0.0952731109488886</v>
       </c>
       <c r="H6" t="n">
-        <v>-0.23957018479683673</v>
+        <v>-0.0899412790053172</v>
       </c>
       <c r="I6" t="n">
-        <v>-0.5454789416164917</v>
+        <v>-0.526709423475617</v>
       </c>
       <c r="J6" t="n">
-        <v>-0.3293321552291316</v>
+        <v>-0.1103014664983646</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.3888470226485382</v>
+        <v>-0.19399745402978058</v>
       </c>
       <c r="L6" t="n">
-        <v>0.3595079448354044</v>
+        <v>0.3426919865702904</v>
       </c>
       <c r="M6" t="n">
-        <v>0.13762064075119676</v>
+        <v>0.1152803274035806</v>
       </c>
       <c r="N6" t="n">
-        <v>0.03789353396774027</v>
+        <v>-0.14641542585978565</v>
       </c>
       <c r="O6" t="n">
-        <v>-0.031930771919211134</v>
+        <v>-0.16377208765088283</v>
       </c>
       <c r="P6" t="n">
-        <v>0.004666037754354639</v>
+        <v>-0.07047626535477734</v>
       </c>
       <c r="Q6" t="n">
-        <v>-0.10948085814489904</v>
+        <v>-0.17371263753628233</v>
       </c>
       <c r="R6" t="n">
-        <v>0.6464985109994327</v>
+        <v>0.2936399899923804</v>
       </c>
       <c r="S6" t="n">
-        <v>0.8008145288142814</v>
+        <v>0.4794744558722764</v>
       </c>
       <c r="T6" t="n">
-        <v>0.8280194468046549</v>
+        <v>0.6621609361454874</v>
       </c>
       <c r="U6" t="n">
-        <v>0.5091880490331859</v>
+        <v>0.7163129219507298</v>
       </c>
       <c r="V6" t="n">
-        <v>0.388665619258127</v>
+        <v>0.6115701807418943</v>
       </c>
       <c r="W6" t="n">
-        <v>0.16591617256848587</v>
+        <v>0.42988931277722886</v>
       </c>
       <c r="X6" t="n">
-        <v>0.6153168951501158</v>
+        <v>0.7069934003204769</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.6800889735072642</v>
+        <v>0.5876551346638111</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.525643539898449</v>
+        <v>0.8164027659474693</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.45403232691030493</v>
+        <v>0.9012162016396166</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.3674484769693176</v>
+        <v>-0.3845642764798581</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.4148863396508286</v>
+        <v>-0.45807287487611686</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.44442827223672765</v>
+        <v>-0.46586928425230273</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.45872576548696536</v>
+        <v>-0.49273102936503754</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.4074394917428705</v>
+        <v>-0.4398591697938615</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.34426375972054285</v>
+        <v>-0.2682003345073521</v>
       </c>
       <c r="H7" t="n">
-        <v>-0.39905456424006586</v>
+        <v>-0.3534323366052071</v>
       </c>
       <c r="I7" t="n">
-        <v>-0.5309385020499501</v>
+        <v>-0.5532472488792809</v>
       </c>
       <c r="J7" t="n">
-        <v>-0.25662829203818827</v>
+        <v>-0.0889568185956354</v>
       </c>
       <c r="K7" t="n">
-        <v>-0.17145352793091623</v>
+        <v>-0.004921107229130071</v>
       </c>
       <c r="L7" t="n">
-        <v>0.6083174694893678</v>
+        <v>0.5674797048208979</v>
       </c>
       <c r="M7" t="n">
-        <v>0.39196593065624125</v>
+        <v>0.33005183500503726</v>
       </c>
       <c r="N7" t="n">
-        <v>0.06391993675554226</v>
+        <v>-0.08209173516436569</v>
       </c>
       <c r="O7" t="n">
-        <v>-0.006235097405211482</v>
+        <v>-0.014841849893591148</v>
       </c>
       <c r="P7" t="n">
-        <v>0.18697714163425466</v>
+        <v>0.15198817583939123</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.12867962167527558</v>
+        <v>0.0744814078136106</v>
       </c>
       <c r="R7" t="n">
-        <v>0.8665530944058365</v>
+        <v>-0.027968347361823177</v>
       </c>
       <c r="S7" t="n">
-        <v>0.5768232432398408</v>
+        <v>-0.01691496750465186</v>
       </c>
       <c r="T7" t="n">
-        <v>0.5552382012163971</v>
+        <v>0.08971608428587463</v>
       </c>
       <c r="U7" t="n">
-        <v>0.4151124006195333</v>
+        <v>0.23265729511907196</v>
       </c>
       <c r="V7" t="n">
-        <v>0.13785297998030008</v>
+        <v>0.2373961248052734</v>
       </c>
       <c r="W7" t="n">
-        <v>-0.06627651197598783</v>
+        <v>0.19990160769794757</v>
       </c>
       <c r="X7" t="n">
-        <v>0.10798235606006677</v>
+        <v>0.8969232099474853</v>
       </c>
       <c r="Y7" t="n">
-        <v>0.2026553324080775</v>
+        <v>0.5173014910920428</v>
       </c>
       <c r="Z7" t="n">
-        <v>0.18364768666819292</v>
+        <v>0.646358282976045</v>
       </c>
       <c r="AA7" t="n">
-        <v>-0.011985416950184997</v>
+        <v>0.6032227108083275</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.2587599511281767</v>
+        <v>-0.2951722209489358</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.02001797182390292</v>
+        <v>6.388362466388666E-5</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.015601902147113775</v>
+        <v>0.024673447365654477</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.12918522658416698</v>
+        <v>-0.12070103213703796</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.16249434270772536</v>
+        <v>-0.12989036264062287</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.5120961512536611</v>
+        <v>-0.6367928986251561</v>
       </c>
       <c r="H8" t="n">
-        <v>-0.4964911389204811</v>
+        <v>-0.5980724966274987</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.41289238462365596</v>
+        <v>-0.4425383802497762</v>
       </c>
       <c r="J8" t="n">
-        <v>-0.5766071749565815</v>
+        <v>-0.679439173272901</v>
       </c>
       <c r="K8" t="n">
-        <v>-0.42192525746913745</v>
+        <v>-0.5571791944140349</v>
       </c>
       <c r="L8" t="n">
-        <v>0.5807745680396651</v>
+        <v>0.6413186020549244</v>
       </c>
       <c r="M8" t="n">
-        <v>0.7336053730642179</v>
+        <v>0.8052684685924324</v>
       </c>
       <c r="N8" t="n">
-        <v>0.6151015528225598</v>
+        <v>0.5919047661162683</v>
       </c>
       <c r="O8" t="n">
-        <v>0.5605353675366922</v>
+        <v>0.7609514443888198</v>
       </c>
       <c r="P8" t="n">
-        <v>0.7049503773840263</v>
+        <v>0.7889927520092334</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.8128813291019908</v>
+        <v>0.8608726571100122</v>
       </c>
       <c r="R8" t="n">
-        <v>0.14062862472119494</v>
+        <v>-0.47132422912191346</v>
       </c>
       <c r="S8" t="n">
-        <v>-0.15583316534120303</v>
+        <v>-0.5140858223619288</v>
       </c>
       <c r="T8" t="n">
-        <v>-0.029641235141088684</v>
+        <v>-0.37950218491642623</v>
       </c>
       <c r="U8" t="n">
-        <v>-0.13604740262403028</v>
+        <v>-0.4619056440725787</v>
       </c>
       <c r="V8" t="n">
-        <v>0.13915751961372982</v>
+        <v>-0.4613353113355014</v>
       </c>
       <c r="W8" t="n">
-        <v>-0.3871636725654482</v>
+        <v>0.28811767752655454</v>
       </c>
       <c r="X8" t="n">
-        <v>-0.2733815483490167</v>
+        <v>0.09272434135338654</v>
       </c>
       <c r="Y8" t="n">
-        <v>-0.3615398459580121</v>
+        <v>-0.19592365705454115</v>
       </c>
       <c r="Z8" t="n">
-        <v>-0.3666868568811769</v>
+        <v>-0.259237310701704</v>
       </c>
       <c r="AA8" t="n">
-        <v>-0.4365231027423483</v>
+        <v>-0.11058796588799372</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated outputs after afd2073c
</commit_message>
<xml_diff>
--- a/processed-data/rdata/spe/08_spatial_registration/bayesSpace_layer_cor_annotations.xlsx
+++ b/processed-data/rdata/spe/08_spatial_registration/bayesSpace_layer_cor_annotations.xlsx
@@ -8,8 +8,8 @@
   <sheets>
     <sheet name="Key" r:id="rId3" sheetId="1"/>
     <sheet name="annotation" r:id="rId4" sheetId="2"/>
-    <sheet name="cor_k7" r:id="rId5" sheetId="3"/>
-    <sheet name="cor_k9" r:id="rId6" sheetId="4"/>
+    <sheet name="cor_k07" r:id="rId5" sheetId="3"/>
+    <sheet name="cor_k09" r:id="rId6" sheetId="4"/>
     <sheet name="cor_k16" r:id="rId7" sheetId="5"/>
     <sheet name="cor_k28" r:id="rId8" sheetId="6"/>
   </sheets>
@@ -28,10 +28,10 @@
     <t>annotation</t>
   </si>
   <si>
-    <t>cor_k7</t>
-  </si>
-  <si>
-    <t>cor_k9</t>
+    <t>cor_k07</t>
+  </si>
+  <si>
+    <t>cor_k09</t>
   </si>
   <si>
     <t>cor_k16</t>
@@ -43,10 +43,10 @@
     <t>Annotations of baySpace Domains</t>
   </si>
   <si>
-    <t>Correlation values vs. manual annotation for k7</t>
-  </si>
-  <si>
-    <t>Correlation values vs. manual annotation for k9</t>
+    <t>Correlation values vs. manual annotation for k07</t>
+  </si>
+  <si>
+    <t>Correlation values vs. manual annotation for k09</t>
   </si>
   <si>
     <t>Correlation values vs. manual annotation for k16</t>

</xml_diff>

<commit_message>
Also update table outputs after 4d1d3588
</commit_message>
<xml_diff>
--- a/processed-data/rdata/spe/08_spatial_registration/bayesSpace_layer_cor_annotations.xlsx
+++ b/processed-data/rdata/spe/08_spatial_registration/bayesSpace_layer_cor_annotations.xlsx
@@ -8,16 +8,17 @@
   <sheets>
     <sheet name="Key" r:id="rId3" sheetId="1"/>
     <sheet name="annotation" r:id="rId4" sheetId="2"/>
-    <sheet name="cor_k07" r:id="rId5" sheetId="3"/>
-    <sheet name="cor_k09" r:id="rId6" sheetId="4"/>
-    <sheet name="cor_k16" r:id="rId7" sheetId="5"/>
-    <sheet name="cor_k28" r:id="rId8" sheetId="6"/>
+    <sheet name="cor_k02" r:id="rId5" sheetId="3"/>
+    <sheet name="cor_k07" r:id="rId6" sheetId="4"/>
+    <sheet name="cor_k09" r:id="rId7" sheetId="5"/>
+    <sheet name="cor_k16" r:id="rId8" sheetId="6"/>
+    <sheet name="cor_k28" r:id="rId9" sheetId="7"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="228">
   <si>
     <t>data</t>
   </si>
@@ -28,6 +29,9 @@
     <t>annotation</t>
   </si>
   <si>
+    <t>cor_k02</t>
+  </si>
+  <si>
     <t>cor_k07</t>
   </si>
   <si>
@@ -43,6 +47,9 @@
     <t>Annotations of baySpace Domains</t>
   </si>
   <si>
+    <t>Correlation values vs. manual annotation for k02</t>
+  </si>
+  <si>
     <t>Correlation values vs. manual annotation for k07</t>
   </si>
   <si>
@@ -76,6 +83,12 @@
     <t>layer_label</t>
   </si>
   <si>
+    <t>L3</t>
+  </si>
+  <si>
+    <t>WM</t>
+  </si>
+  <si>
     <t>L1</t>
   </si>
   <si>
@@ -91,24 +104,24 @@
     <t>L6</t>
   </si>
   <si>
-    <t>WM</t>
-  </si>
-  <si>
-    <t>L3</t>
+    <t>L2</t>
   </si>
   <si>
     <t>L4</t>
   </si>
   <si>
-    <t>L2</t>
-  </si>
-  <si>
     <t>L5/6</t>
   </si>
   <si>
     <t>L6/WM</t>
   </si>
   <si>
+    <t>Sp02D02 ~ L3</t>
+  </si>
+  <si>
+    <t>Sp02D01 ~ WM</t>
+  </si>
+  <si>
     <t>Sp07D01 ~ L1</t>
   </si>
   <si>
@@ -136,7 +149,7 @@
     <t>Sp09D02 ~ L1</t>
   </si>
   <si>
-    <t>Sp09D03 ~ L2/3</t>
+    <t>Sp09D03 ~ L2</t>
   </si>
   <si>
     <t>Sp09D05 ~ L3</t>
@@ -283,6 +296,12 @@
     <t>Sp28D28 ~ WM</t>
   </si>
   <si>
+    <t>L3 Sp02D02</t>
+  </si>
+  <si>
+    <t>WM Sp02D01</t>
+  </si>
+  <si>
     <t>L1 Sp07D01</t>
   </si>
   <si>
@@ -310,7 +329,7 @@
     <t>L1 Sp09D02</t>
   </si>
   <si>
-    <t>L2/3 Sp09D03</t>
+    <t>L2 Sp09D03</t>
   </si>
   <si>
     <t>L3 Sp09D05</t>
@@ -457,6 +476,9 @@
     <t>WM Sp28D28</t>
   </si>
   <si>
+    <t>k02</t>
+  </si>
+  <si>
     <t>k07</t>
   </si>
   <si>
@@ -467,6 +489,12 @@
   </si>
   <si>
     <t>k28</t>
+  </si>
+  <si>
+    <t>Sp02D02</t>
+  </si>
+  <si>
+    <t>Sp02D01</t>
   </si>
   <si>
     <t>Sp07D01</t>
@@ -737,7 +765,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">
@@ -745,7 +773,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4">
@@ -753,7 +781,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
@@ -761,7 +789,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6">
@@ -769,7 +797,15 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -787,1014 +823,1014 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="D2" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="E2" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="F2" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D3" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="E3" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="F3" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="D4" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="E4" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="F4" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G4" t="s">
-        <v>209</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D5" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="E5" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="F5" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="D6" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="E6" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="F6" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G6" t="s">
-        <v>23</v>
+        <v>218</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D7" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="E7" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="F7" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="D8" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="E8" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="F8" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G8" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="D9" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="E9" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="F9" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G9" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="D10" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="E10" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="F10" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G10" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="D11" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="E11" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="F11" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G11" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="D12" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="E12" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="F12" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="D13" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="E13" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="F13" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G13" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C14" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D14" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="E14" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="F14" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D15" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="E15" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="F15" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G15" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D16" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="E16" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="F16" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G16" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C17" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="D17" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="E17" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="F17" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G17" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C18" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D18" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="E18" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="F18" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G18" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C19" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="D19" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="E19" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="F19" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G19" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C20" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="D20" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="E20" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="F20" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G20" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C21" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="D21" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="E21" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="F21" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G21" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C22" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D22" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="E22" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="F22" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G22" t="s">
-        <v>210</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C23" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D23" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="E23" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="F23" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G23" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C24" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="D24" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="E24" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="F24" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G24" t="s">
-        <v>209</v>
+        <v>219</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C25" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="D25" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="E25" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="F25" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G25" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C26" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D26" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="E26" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="F26" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G26" t="s">
-        <v>22</v>
+        <v>218</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C27" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="D27" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="E27" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="F27" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G27" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C28" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="D28" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="E28" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="F28" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G28" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C29" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D29" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="E29" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="F29" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G29" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C30" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D30" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="E30" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="F30" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G30" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B31" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C31" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="D31" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="E31" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="F31" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G31" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B32" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C32" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D32" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="E32" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="F32" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G32" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B33" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C33" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="D33" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="E33" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="F33" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G33" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B34" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C34" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D34" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="E34" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="F34" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G34" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B35" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C35" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="D35" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="E35" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="F35" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G35" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B36" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C36" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="D36" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="E36" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="F36" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G36" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B37" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C37" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="D37" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="E37" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="F37" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G37" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B38" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C38" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="D38" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="E38" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="F38" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G38" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B39" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C39" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="D39" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="E39" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="F39" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G39" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B40" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C40" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="D40" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="E40" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="F40" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G40" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B41" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C41" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="D41" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="E41" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="F41" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G41" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B42" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C42" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="D42" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="E42" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="F42" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G42" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B43" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C43" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="D43" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="E43" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="F43" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G43" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B44" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C44" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="D44" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="E44" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="F44" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G44" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="45">
@@ -1802,22 +1838,22 @@
         <v>21</v>
       </c>
       <c r="B45" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C45" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="D45" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="E45" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="F45" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G45" t="s">
-        <v>209</v>
+        <v>21</v>
       </c>
     </row>
     <row r="46">
@@ -1825,321 +1861,367 @@
         <v>21</v>
       </c>
       <c r="B46" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C46" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="D46" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="E46" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="F46" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G46" t="s">
-        <v>209</v>
+        <v>21</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B47" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C47" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D47" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="E47" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
       <c r="F47" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G47" t="s">
-        <v>26</v>
+        <v>218</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B48" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C48" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="D48" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="E48" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="F48" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G48" t="s">
-        <v>26</v>
+        <v>218</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B49" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C49" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="D49" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="E49" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="F49" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G49" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B50" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C50" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="D50" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="E50" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="F50" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G50" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B51" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C51" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="D51" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="E51" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="F51" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G51" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B52" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C52" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="D52" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="E52" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="F52" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G52" t="s">
-        <v>211</v>
+        <v>26</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B53" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C53" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="D53" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="E53" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="F53" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G53" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B54" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C54" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="D54" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="E54" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="F54" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G54" t="s">
-        <v>23</v>
+        <v>220</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B55" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C55" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="D55" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="E55" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="F55" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G55" t="s">
-        <v>212</v>
+        <v>27</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B56" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C56" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="D56" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="E56" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="F56" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G56" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B57" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C57" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="D57" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="E57" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="F57" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G57" t="s">
-        <v>24</v>
+        <v>221</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B58" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C58" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="D58" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="E58" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="F58" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G58" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B59" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C59" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D59" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="E59" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
       <c r="F59" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G59" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>22</v>
+      </c>
+      <c r="B60" t="s">
+        <v>90</v>
+      </c>
+      <c r="C60" t="s">
+        <v>150</v>
+      </c>
+      <c r="D60" t="s">
+        <v>156</v>
+      </c>
+      <c r="E60" t="s">
+        <v>215</v>
+      </c>
+      <c r="F60" t="s">
+        <v>217</v>
+      </c>
+      <c r="G60" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>22</v>
+      </c>
+      <c r="B61" t="s">
+        <v>91</v>
+      </c>
+      <c r="C61" t="s">
+        <v>151</v>
+      </c>
+      <c r="D61" t="s">
+        <v>156</v>
+      </c>
+      <c r="E61" t="s">
+        <v>216</v>
+      </c>
+      <c r="F61" t="s">
+        <v>217</v>
+      </c>
+      <c r="G61" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -2158,207 +2240,87 @@
     <row r="1">
       <c r="A1"/>
       <c r="B1" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="C1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D1" t="s">
-        <v>156</v>
-      </c>
-      <c r="E1" t="s">
-        <v>151</v>
-      </c>
-      <c r="F1" t="s">
-        <v>152</v>
-      </c>
-      <c r="G1" t="s">
-        <v>153</v>
-      </c>
-      <c r="H1" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2" t="n">
-        <v>0.08660062969117822</v>
+        <v>0.946137198670078</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9456898796852619</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.7857668336202132</v>
-      </c>
-      <c r="E2" t="n">
-        <v>-0.703168222171207</v>
-      </c>
-      <c r="F2" t="n">
-        <v>-0.7304689702950955</v>
-      </c>
-      <c r="G2" t="n">
-        <v>-0.4405351412196086</v>
-      </c>
-      <c r="H2" t="n">
-        <v>-0.16357202679915997</v>
+        <v>-0.946137198670078</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.4340853700232825</v>
+        <v>0.15085424363618674</v>
       </c>
       <c r="C3" t="n">
-        <v>0.14427111663479428</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.28065608542914505</v>
-      </c>
-      <c r="E3" t="n">
-        <v>-0.3456118303240812</v>
-      </c>
-      <c r="F3" t="n">
-        <v>-0.350131745075143</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.17716847094818242</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.8703054108497322</v>
+        <v>-0.15085424363618685</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.5086105497177728</v>
+        <v>-0.2982807353426284</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.22259257788519182</v>
-      </c>
-      <c r="D4" t="n">
-        <v>-0.12706790495966055</v>
-      </c>
-      <c r="E4" t="n">
-        <v>-0.28421407307668256</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.2309750168074776</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0.9009592363368231</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0.3433636015349134</v>
+        <v>0.29828073534262844</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.3521447758367443</v>
+        <v>-0.5470939684763435</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.420832961573367</v>
-      </c>
-      <c r="D5" t="n">
-        <v>-0.4574811494505126</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.11556203304777851</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.8088068215916977</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0.5758024008267725</v>
-      </c>
-      <c r="H5" t="n">
-        <v>-0.11240526294299671</v>
+        <v>0.5470939684763437</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.010171671637480926</v>
+        <v>-0.7006920627120939</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.6588935627231943</v>
-      </c>
-      <c r="D6" t="n">
-        <v>-0.6533933751430407</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.8317515738333782</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.7488153111236104</v>
-      </c>
-      <c r="G6" t="n">
-        <v>-0.025509865767148365</v>
-      </c>
-      <c r="H6" t="n">
-        <v>-0.23060036504821907</v>
+        <v>0.7006920627120939</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="B7" t="n">
-        <v>0.15585493201312609</v>
+        <v>-0.4342991243195949</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.46911493039457136</v>
-      </c>
-      <c r="D7" t="n">
-        <v>-0.41956421431437546</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.841837149022825</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0.18980459237037614</v>
-      </c>
-      <c r="G7" t="n">
-        <v>-0.2927599907305512</v>
-      </c>
-      <c r="H7" t="n">
-        <v>-0.06348084812420124</v>
+        <v>0.4342991243195946</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
       <c r="B8" t="n">
-        <v>0.9093240054734891</v>
+        <v>0.12022817205408161</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.03136033444546572</v>
-      </c>
-      <c r="D8" t="n">
-        <v>-0.024815451015961963</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0.1325671450562423</v>
-      </c>
-      <c r="F8" t="n">
-        <v>-0.2681293810616702</v>
-      </c>
-      <c r="G8" t="n">
-        <v>-0.545656476613206</v>
-      </c>
-      <c r="H8" t="n">
-        <v>-0.5413264400619362</v>
+        <v>-0.12022817205408162</v>
       </c>
     </row>
   </sheetData>
@@ -2377,255 +2339,207 @@
     <row r="1">
       <c r="A1"/>
       <c r="B1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C1" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="D1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E1" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="F1" t="s">
+        <v>161</v>
+      </c>
+      <c r="G1" t="s">
         <v>162</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>163</v>
-      </c>
-      <c r="H1" t="s">
-        <v>159</v>
-      </c>
-      <c r="I1" t="s">
-        <v>160</v>
-      </c>
-      <c r="J1" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2" t="n">
-        <v>0.18233409248506321</v>
+        <v>0.08660062969117822</v>
       </c>
       <c r="C2" t="n">
-        <v>0.10116109321566395</v>
+        <v>0.9456898796852619</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9452202433345341</v>
+        <v>0.7857668336202132</v>
       </c>
       <c r="E2" t="n">
-        <v>0.8038452401893256</v>
+        <v>-0.703168222171207</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.3756919512330929</v>
+        <v>-0.7304689702950955</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.1819621162663477</v>
+        <v>-0.4405351412196086</v>
       </c>
       <c r="H2" t="n">
-        <v>-0.6340380051280985</v>
-      </c>
-      <c r="I2" t="n">
-        <v>-0.7940434813686468</v>
-      </c>
-      <c r="J2" t="n">
-        <v>-0.6286441496949572</v>
+        <v>-0.16357202679915997</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.28515927125845497</v>
+        <v>-0.4340853700232825</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.3742808103087616</v>
+        <v>0.14427111663479428</v>
       </c>
       <c r="D3" t="n">
-        <v>0.13145478640958205</v>
+        <v>0.28065608542914505</v>
       </c>
       <c r="E3" t="n">
-        <v>0.5302265400880759</v>
+        <v>-0.3456118303240812</v>
       </c>
       <c r="F3" t="n">
-        <v>0.2503070267569068</v>
+        <v>-0.350131745075143</v>
       </c>
       <c r="G3" t="n">
-        <v>0.8631575902918986</v>
+        <v>0.17716847094818242</v>
       </c>
       <c r="H3" t="n">
-        <v>-0.267699954622677</v>
-      </c>
-      <c r="I3" t="n">
-        <v>-0.33654306413292895</v>
-      </c>
-      <c r="J3" t="n">
-        <v>-0.22786700724759576</v>
+        <v>0.8703054108497322</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.34484934977670956</v>
+        <v>-0.5086105497177728</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.4862492001819124</v>
+        <v>-0.22259257788519182</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.19214050745655667</v>
+        <v>-0.12706790495966055</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.04815214362516406</v>
+        <v>-0.28421407307668256</v>
       </c>
       <c r="F4" t="n">
-        <v>0.9257536491525145</v>
+        <v>0.2309750168074776</v>
       </c>
       <c r="G4" t="n">
-        <v>0.4172568716280277</v>
+        <v>0.9009592363368231</v>
       </c>
       <c r="H4" t="n">
-        <v>-0.30703556687043404</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0.04368405258338519</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0.38992075891358086</v>
+        <v>0.3433636015349134</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.28101291175617527</v>
+        <v>-0.3521447758367443</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.3986331047681389</v>
+        <v>-0.420832961573367</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.3962732830634432</v>
+        <v>-0.4574811494505126</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.5272924111084012</v>
+        <v>0.11556203304777851</v>
       </c>
       <c r="F5" t="n">
-        <v>0.5492681141632048</v>
+        <v>0.8088068215916977</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.03938880566569008</v>
+        <v>0.5758024008267725</v>
       </c>
       <c r="H5" t="n">
-        <v>0.002362978231716639</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0.5692207638043618</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0.886617952543041</v>
+        <v>-0.11240526294299671</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.11403512224647375</v>
+        <v>-0.010171671637480926</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.06103860756914444</v>
+        <v>-0.6588935627231943</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.665129523126223</v>
+        <v>-0.6533933751430407</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.7583633314635398</v>
+        <v>0.8317515738333782</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.08857852853631731</v>
+        <v>0.7488153111236104</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.23049140606647356</v>
+        <v>-0.025509865767148365</v>
       </c>
       <c r="H6" t="n">
-        <v>0.7563890580955026</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0.8972083564188468</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0.5874068204253086</v>
+        <v>-0.23060036504821907</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.0454523774864195</v>
+        <v>0.15585493201312609</v>
       </c>
       <c r="C7" t="n">
-        <v>0.17502466270998837</v>
+        <v>-0.46911493039457136</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.48744631958558693</v>
+        <v>-0.41956421431437546</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.42804452746699106</v>
+        <v>0.841837149022825</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.32876891000139147</v>
+        <v>0.18980459237037614</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.09099482789754662</v>
+        <v>-0.2927599907305512</v>
       </c>
       <c r="H7" t="n">
-        <v>0.8922991320258268</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0.49706489375206103</v>
-      </c>
-      <c r="J7" t="n">
-        <v>-0.0061334148746578585</v>
+        <v>-0.06348084812420124</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
       <c r="B8" t="n">
-        <v>0.6747530442684894</v>
+        <v>0.9093240054734891</v>
       </c>
       <c r="C8" t="n">
-        <v>0.8700732349717306</v>
+        <v>-0.03136033444546572</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.047160066578838145</v>
+        <v>-0.024815451015961963</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.20522960157831152</v>
+        <v>0.1325671450562423</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.6114803315484088</v>
+        <v>-0.2681293810616702</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.6035094347578965</v>
+        <v>-0.545656476613206</v>
       </c>
       <c r="H8" t="n">
-        <v>0.08707286710222814</v>
-      </c>
-      <c r="I8" t="n">
-        <v>-0.19646796554293255</v>
-      </c>
-      <c r="J8" t="n">
-        <v>-0.43881914191839133</v>
+        <v>-0.5413264400619362</v>
       </c>
     </row>
   </sheetData>
@@ -2650,417 +2564,249 @@
         <v>167</v>
       </c>
       <c r="D1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G1" t="s">
+        <v>172</v>
+      </c>
+      <c r="H1" t="s">
         <v>168</v>
       </c>
-      <c r="E1" t="s">
-        <v>178</v>
-      </c>
-      <c r="F1" t="s">
-        <v>181</v>
-      </c>
-      <c r="G1" t="s">
-        <v>179</v>
-      </c>
-      <c r="H1" t="s">
-        <v>180</v>
-      </c>
       <c r="I1" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="J1" t="s">
-        <v>175</v>
-      </c>
-      <c r="K1" t="s">
-        <v>176</v>
-      </c>
-      <c r="L1" t="s">
-        <v>177</v>
-      </c>
-      <c r="M1" t="s">
-        <v>173</v>
-      </c>
-      <c r="N1" t="s">
-        <v>172</v>
-      </c>
-      <c r="O1" t="s">
-        <v>171</v>
-      </c>
-      <c r="P1" t="s">
-        <v>169</v>
-      </c>
-      <c r="Q1" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2" t="n">
-        <v>0.10623370693351285</v>
+        <v>0.18233409248506321</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.08267214344632225</v>
+        <v>0.10116109321566395</v>
       </c>
       <c r="D2" t="n">
-        <v>0.13769859508135188</v>
+        <v>0.9452202433345341</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9324690598162875</v>
+        <v>0.8038452401893256</v>
       </c>
       <c r="F2" t="n">
-        <v>0.9376035235564886</v>
+        <v>-0.3756919512330929</v>
       </c>
       <c r="G2" t="n">
-        <v>0.7612907705281787</v>
+        <v>-0.1819621162663477</v>
       </c>
       <c r="H2" t="n">
-        <v>0.7078324597805657</v>
+        <v>-0.6340380051280985</v>
       </c>
       <c r="I2" t="n">
-        <v>-0.46304116555464747</v>
+        <v>-0.7940434813686468</v>
       </c>
       <c r="J2" t="n">
-        <v>-0.4293173486036175</v>
-      </c>
-      <c r="K2" t="n">
-        <v>-0.3069206290113158</v>
-      </c>
-      <c r="L2" t="n">
-        <v>-0.07529462489672085</v>
-      </c>
-      <c r="M2" t="n">
-        <v>-0.6739087409765425</v>
-      </c>
-      <c r="N2" t="n">
-        <v>-0.725204189539131</v>
-      </c>
-      <c r="O2" t="n">
-        <v>-0.812447350558036</v>
-      </c>
-      <c r="P2" t="n">
-        <v>-0.6719594424325679</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>-0.5744331439226147</v>
+        <v>-0.6286441496949572</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.2837111938160821</v>
+        <v>-0.28515927125845497</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.392003544371284</v>
+        <v>-0.3742808103087616</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.38218522595491855</v>
+        <v>0.13145478640958205</v>
       </c>
       <c r="E3" t="n">
-        <v>0.03986185832164309</v>
+        <v>0.5302265400880759</v>
       </c>
       <c r="F3" t="n">
-        <v>0.19095028805064332</v>
+        <v>0.2503070267569068</v>
       </c>
       <c r="G3" t="n">
-        <v>0.32182396105397765</v>
+        <v>0.8631575902918986</v>
       </c>
       <c r="H3" t="n">
-        <v>0.6057401648062378</v>
+        <v>-0.267699954622677</v>
       </c>
       <c r="I3" t="n">
-        <v>0.2846453282564251</v>
+        <v>-0.33654306413292895</v>
       </c>
       <c r="J3" t="n">
-        <v>0.17321455585679027</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0.8162905523842747</v>
-      </c>
-      <c r="L3" t="n">
-        <v>0.617942524720362</v>
-      </c>
-      <c r="M3" t="n">
-        <v>-0.2396867952985173</v>
-      </c>
-      <c r="N3" t="n">
-        <v>-0.19753879859134477</v>
-      </c>
-      <c r="O3" t="n">
-        <v>-0.32937848397777025</v>
-      </c>
-      <c r="P3" t="n">
-        <v>-0.23322485774539362</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>-0.24994909738262677</v>
+        <v>-0.22786700724759576</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.32280653004805304</v>
+        <v>-0.34484934977670956</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.47502254054936754</v>
+        <v>-0.4862492001819124</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.5084873185555933</v>
+        <v>-0.19214050745655667</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.2733598559532801</v>
+        <v>-0.04815214362516406</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.20314592099261913</v>
+        <v>0.9257536491525145</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.07545417958075823</v>
+        <v>0.4172568716280277</v>
       </c>
       <c r="H4" t="n">
-        <v>0.014923159118625406</v>
+        <v>-0.30703556687043404</v>
       </c>
       <c r="I4" t="n">
-        <v>0.8874504552207647</v>
+        <v>0.04368405258338519</v>
       </c>
       <c r="J4" t="n">
-        <v>0.8698882418309373</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0.39056696759828224</v>
-      </c>
-      <c r="L4" t="n">
-        <v>0.5053578630351848</v>
-      </c>
-      <c r="M4" t="n">
-        <v>0.35631939341537733</v>
-      </c>
-      <c r="N4" t="n">
-        <v>0.30409683145337446</v>
-      </c>
-      <c r="O4" t="n">
-        <v>-0.003941282239027194</v>
-      </c>
-      <c r="P4" t="n">
-        <v>-0.25896577305422697</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>-0.08902828657016719</v>
+        <v>0.38992075891358086</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.2454755697579533</v>
+        <v>-0.28101291175617527</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.3473049878491409</v>
+        <v>-0.3986331047681389</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.38873652749128407</v>
+        <v>-0.3962732830634432</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.3979726995545743</v>
+        <v>-0.5272924111084012</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.4649964571489065</v>
+        <v>0.5492681141632048</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.4054796399824032</v>
+        <v>-0.03938880566569008</v>
       </c>
       <c r="H5" t="n">
-        <v>-0.47883394208385666</v>
+        <v>0.002362978231716639</v>
       </c>
       <c r="I5" t="n">
-        <v>0.5316789386151662</v>
+        <v>0.5692207638043618</v>
       </c>
       <c r="J5" t="n">
-        <v>0.6218039149229553</v>
-      </c>
-      <c r="K5" t="n">
-        <v>-0.025760252710276422</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0.04411911782137132</v>
-      </c>
-      <c r="M5" t="n">
-        <v>0.8560078210346629</v>
-      </c>
-      <c r="N5" t="n">
-        <v>0.7693205632963193</v>
-      </c>
-      <c r="O5" t="n">
-        <v>0.5034141524562444</v>
-      </c>
-      <c r="P5" t="n">
-        <v>0.04985451502705304</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>0.17256725714162546</v>
+        <v>0.886617952543041</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.05692450410370169</v>
+        <v>-0.11403512224647375</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0912562227471629</v>
+        <v>-0.06103860756914444</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.06694183136595373</v>
+        <v>-0.665129523126223</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.6202345203562702</v>
+        <v>-0.7583633314635398</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.7032023237585672</v>
+        <v>-0.08857852853631731</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.662160496752198</v>
+        <v>-0.23049140606647356</v>
       </c>
       <c r="H6" t="n">
-        <v>-0.7180562095435445</v>
+        <v>0.7563890580955026</v>
       </c>
       <c r="I6" t="n">
-        <v>0.011546289844407087</v>
+        <v>0.8972083564188468</v>
       </c>
       <c r="J6" t="n">
-        <v>0.020808856047984943</v>
-      </c>
-      <c r="K6" t="n">
-        <v>-0.09125144941524208</v>
-      </c>
-      <c r="L6" t="n">
-        <v>-0.3079482774220605</v>
-      </c>
-      <c r="M6" t="n">
-        <v>0.6428869899018458</v>
-      </c>
-      <c r="N6" t="n">
-        <v>0.7143680188331257</v>
-      </c>
-      <c r="O6" t="n">
-        <v>0.9071869801247692</v>
-      </c>
-      <c r="P6" t="n">
-        <v>0.7665889315973625</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>0.5767535452249377</v>
+        <v>0.5874068204253086</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.012669879332764705</v>
+        <v>-0.0454523774864195</v>
       </c>
       <c r="C7" t="n">
-        <v>0.3343551553266733</v>
+        <v>0.17502466270998837</v>
       </c>
       <c r="D7" t="n">
-        <v>0.11608998739760935</v>
+        <v>-0.48744631958558693</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.45811679550048345</v>
+        <v>-0.42804452746699106</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.46552388187428834</v>
+        <v>-0.32876891000139147</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.4391615973711572</v>
+        <v>-0.09099482789754662</v>
       </c>
       <c r="H7" t="n">
-        <v>-0.3996949336958158</v>
+        <v>0.8922991320258268</v>
       </c>
       <c r="I7" t="n">
-        <v>-0.2161283646737019</v>
+        <v>0.49706489375206103</v>
       </c>
       <c r="J7" t="n">
-        <v>-0.27441360724677644</v>
-      </c>
-      <c r="K7" t="n">
-        <v>0.04760049836177583</v>
-      </c>
-      <c r="L7" t="n">
-        <v>-0.30177258344158875</v>
-      </c>
-      <c r="M7" t="n">
-        <v>0.07507506882881715</v>
-      </c>
-      <c r="N7" t="n">
-        <v>0.21811990018049413</v>
-      </c>
-      <c r="O7" t="n">
-        <v>0.5667940580925148</v>
-      </c>
-      <c r="P7" t="n">
-        <v>0.8704932383190563</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>0.5462517820242165</v>
+        <v>-0.0061334148746578585</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
       <c r="B8" t="n">
-        <v>0.6334779047728258</v>
+        <v>0.6747530442684894</v>
       </c>
       <c r="C8" t="n">
-        <v>0.8290645755848722</v>
+        <v>0.8700732349717306</v>
       </c>
       <c r="D8" t="n">
-        <v>0.8603122764633632</v>
+        <v>-0.047160066578838145</v>
       </c>
       <c r="E8" t="n">
-        <v>0.02729586958707751</v>
+        <v>-0.20522960157831152</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.04720643394696053</v>
+        <v>-0.6114803315484088</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.11343473555200607</v>
+        <v>-0.6035094347578965</v>
       </c>
       <c r="H8" t="n">
-        <v>-0.30012264635252617</v>
+        <v>0.08707286710222814</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.6150903434122268</v>
+        <v>-0.19646796554293255</v>
       </c>
       <c r="J8" t="n">
-        <v>-0.5831781917405922</v>
-      </c>
-      <c r="K8" t="n">
-        <v>-0.5602218946720319</v>
-      </c>
-      <c r="L8" t="n">
-        <v>-0.4096405727627279</v>
-      </c>
-      <c r="M8" t="n">
-        <v>-0.3918964107958459</v>
-      </c>
-      <c r="N8" t="n">
-        <v>-0.4109668296023477</v>
-      </c>
-      <c r="O8" t="n">
-        <v>-0.11197886986841137</v>
-      </c>
-      <c r="P8" t="n">
-        <v>0.0633208427593049</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>0.10095846102517224</v>
+        <v>-0.43881914191839133</v>
       </c>
     </row>
   </sheetData>
@@ -3079,87 +2825,522 @@
     <row r="1">
       <c r="A1"/>
       <c r="B1" t="s">
-        <v>203</v>
+        <v>175</v>
       </c>
       <c r="C1" t="s">
-        <v>205</v>
+        <v>176</v>
       </c>
       <c r="D1" t="s">
-        <v>206</v>
+        <v>177</v>
       </c>
       <c r="E1" t="s">
-        <v>204</v>
+        <v>187</v>
       </c>
       <c r="F1" t="s">
-        <v>207</v>
+        <v>190</v>
       </c>
       <c r="G1" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="H1" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="I1" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
       <c r="J1" t="s">
-        <v>201</v>
+        <v>184</v>
       </c>
       <c r="K1" t="s">
-        <v>202</v>
+        <v>185</v>
       </c>
       <c r="L1" t="s">
+        <v>186</v>
+      </c>
+      <c r="M1" t="s">
         <v>182</v>
       </c>
-      <c r="M1" t="s">
-        <v>186</v>
-      </c>
       <c r="N1" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="O1" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="P1" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="Q1" t="s">
-        <v>184</v>
-      </c>
-      <c r="R1" t="s">
-        <v>196</v>
-      </c>
-      <c r="S1" t="s">
-        <v>197</v>
-      </c>
-      <c r="T1" t="s">
-        <v>195</v>
-      </c>
-      <c r="U1" t="s">
-        <v>193</v>
-      </c>
-      <c r="V1" t="s">
-        <v>194</v>
-      </c>
-      <c r="W1" t="s">
-        <v>192</v>
-      </c>
-      <c r="X1" t="s">
-        <v>188</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>189</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>190</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.10623370693351285</v>
+      </c>
+      <c r="C2" t="n">
+        <v>-0.08267214344632225</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.13769859508135188</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.9324690598162875</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.9376035235564886</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.7612907705281787</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.7078324597805657</v>
+      </c>
+      <c r="I2" t="n">
+        <v>-0.46304116555464747</v>
+      </c>
+      <c r="J2" t="n">
+        <v>-0.4293173486036175</v>
+      </c>
+      <c r="K2" t="n">
+        <v>-0.3069206290113158</v>
+      </c>
+      <c r="L2" t="n">
+        <v>-0.07529462489672085</v>
+      </c>
+      <c r="M2" t="n">
+        <v>-0.6739087409765425</v>
+      </c>
+      <c r="N2" t="n">
+        <v>-0.725204189539131</v>
+      </c>
+      <c r="O2" t="n">
+        <v>-0.812447350558036</v>
+      </c>
+      <c r="P2" t="n">
+        <v>-0.6719594424325679</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>-0.5744331439226147</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>222</v>
+      </c>
+      <c r="B3" t="n">
+        <v>-0.2837111938160821</v>
+      </c>
+      <c r="C3" t="n">
+        <v>-0.392003544371284</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-0.38218522595491855</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.03986185832164309</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.19095028805064332</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.32182396105397765</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.6057401648062378</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.2846453282564251</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.17321455585679027</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.8162905523842747</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.617942524720362</v>
+      </c>
+      <c r="M3" t="n">
+        <v>-0.2396867952985173</v>
+      </c>
+      <c r="N3" t="n">
+        <v>-0.19753879859134477</v>
+      </c>
+      <c r="O3" t="n">
+        <v>-0.32937848397777025</v>
+      </c>
+      <c r="P3" t="n">
+        <v>-0.23322485774539362</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>-0.24994909738262677</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>223</v>
+      </c>
+      <c r="B4" t="n">
+        <v>-0.32280653004805304</v>
+      </c>
+      <c r="C4" t="n">
+        <v>-0.47502254054936754</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-0.5084873185555933</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-0.2733598559532801</v>
+      </c>
+      <c r="F4" t="n">
+        <v>-0.20314592099261913</v>
+      </c>
+      <c r="G4" t="n">
+        <v>-0.07545417958075823</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.014923159118625406</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.8874504552207647</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.8698882418309373</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.39056696759828224</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.5053578630351848</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.35631939341537733</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.30409683145337446</v>
+      </c>
+      <c r="O4" t="n">
+        <v>-0.003941282239027194</v>
+      </c>
+      <c r="P4" t="n">
+        <v>-0.25896577305422697</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>-0.08902828657016719</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>224</v>
+      </c>
+      <c r="B5" t="n">
+        <v>-0.2454755697579533</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-0.3473049878491409</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-0.38873652749128407</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-0.3979726995545743</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-0.4649964571489065</v>
+      </c>
+      <c r="G5" t="n">
+        <v>-0.4054796399824032</v>
+      </c>
+      <c r="H5" t="n">
+        <v>-0.47883394208385666</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.5316789386151662</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.6218039149229553</v>
+      </c>
+      <c r="K5" t="n">
+        <v>-0.025760252710276422</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.04411911782137132</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.8560078210346629</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.7693205632963193</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.5034141524562444</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0.04985451502705304</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0.17256725714162546</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>225</v>
+      </c>
+      <c r="B6" t="n">
+        <v>-0.05692450410370169</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.0912562227471629</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-0.06694183136595373</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-0.6202345203562702</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-0.7032023237585672</v>
+      </c>
+      <c r="G6" t="n">
+        <v>-0.662160496752198</v>
+      </c>
+      <c r="H6" t="n">
+        <v>-0.7180562095435445</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.011546289844407087</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.020808856047984943</v>
+      </c>
+      <c r="K6" t="n">
+        <v>-0.09125144941524208</v>
+      </c>
+      <c r="L6" t="n">
+        <v>-0.3079482774220605</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.6428869899018458</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.7143680188331257</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.9071869801247692</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.7665889315973625</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0.5767535452249377</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>226</v>
+      </c>
+      <c r="B7" t="n">
+        <v>-0.012669879332764705</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.3343551553266733</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.11608998739760935</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-0.45811679550048345</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-0.46552388187428834</v>
+      </c>
+      <c r="G7" t="n">
+        <v>-0.4391615973711572</v>
+      </c>
+      <c r="H7" t="n">
+        <v>-0.3996949336958158</v>
+      </c>
+      <c r="I7" t="n">
+        <v>-0.2161283646737019</v>
+      </c>
+      <c r="J7" t="n">
+        <v>-0.27441360724677644</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.04760049836177583</v>
+      </c>
+      <c r="L7" t="n">
+        <v>-0.30177258344158875</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.07507506882881715</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.21811990018049413</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.5667940580925148</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0.8704932383190563</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0.5462517820242165</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>227</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.6334779047728258</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.8290645755848722</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.8603122764633632</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.02729586958707751</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-0.04720643394696053</v>
+      </c>
+      <c r="G8" t="n">
+        <v>-0.11343473555200607</v>
+      </c>
+      <c r="H8" t="n">
+        <v>-0.30012264635252617</v>
+      </c>
+      <c r="I8" t="n">
+        <v>-0.6150903434122268</v>
+      </c>
+      <c r="J8" t="n">
+        <v>-0.5831781917405922</v>
+      </c>
+      <c r="K8" t="n">
+        <v>-0.5602218946720319</v>
+      </c>
+      <c r="L8" t="n">
+        <v>-0.4096405727627279</v>
+      </c>
+      <c r="M8" t="n">
+        <v>-0.3918964107958459</v>
+      </c>
+      <c r="N8" t="n">
+        <v>-0.4109668296023477</v>
+      </c>
+      <c r="O8" t="n">
+        <v>-0.11197886986841137</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0.0633208427593049</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>0.10095846102517224</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1"/>
+      <c r="B1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D1" t="s">
+        <v>215</v>
+      </c>
+      <c r="E1" t="s">
+        <v>213</v>
+      </c>
+      <c r="F1" t="s">
+        <v>216</v>
+      </c>
+      <c r="G1" t="s">
+        <v>207</v>
+      </c>
+      <c r="H1" t="s">
+        <v>208</v>
+      </c>
+      <c r="I1" t="s">
+        <v>209</v>
+      </c>
+      <c r="J1" t="s">
+        <v>210</v>
+      </c>
+      <c r="K1" t="s">
+        <v>211</v>
+      </c>
+      <c r="L1" t="s">
+        <v>191</v>
+      </c>
+      <c r="M1" t="s">
+        <v>195</v>
+      </c>
+      <c r="N1" t="s">
+        <v>196</v>
+      </c>
+      <c r="O1" t="s">
+        <v>194</v>
+      </c>
+      <c r="P1" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>193</v>
+      </c>
+      <c r="R1" t="s">
+        <v>205</v>
+      </c>
+      <c r="S1" t="s">
+        <v>206</v>
+      </c>
+      <c r="T1" t="s">
+        <v>204</v>
+      </c>
+      <c r="U1" t="s">
+        <v>202</v>
+      </c>
+      <c r="V1" t="s">
+        <v>203</v>
+      </c>
+      <c r="W1" t="s">
+        <v>201</v>
+      </c>
+      <c r="X1" t="s">
+        <v>197</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>198</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>199</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>22</v>
       </c>
       <c r="B2" t="n">
         <v>0.6785571557691567</v>
@@ -3242,7 +3423,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
       <c r="B3" t="n">
         <v>0.6493644804771322</v>
@@ -3325,7 +3506,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c r="B4" t="n">
         <v>0.03997820409239257</v>
@@ -3408,7 +3589,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="B5" t="n">
         <v>-0.5145619859890052</v>
@@ -3491,7 +3672,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="B6" t="n">
         <v>-0.7232019793467943</v>
@@ -3574,7 +3755,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="B7" t="n">
         <v>-0.3845642764798581</v>
@@ -3657,7 +3838,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
       <c r="B8" t="n">
         <v>-0.2951722209489358</v>

</xml_diff>